<commit_message>
09222220 added review nh wr
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\carbon\my-carbon-site\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\carbon\album_review\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="genesisowusu1" localSheetId="0">Sheet1!$A$1:$E$16</definedName>
-    <definedName name="genesisowusu1" localSheetId="2">Sheet3!$A$1:$E$16</definedName>
+    <definedName name="wrd1_" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
+    <definedName name="wrd1_" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/genesisowusu1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/wrd1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/genesisowusu1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/wrd1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="23">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -75,73 +75,52 @@
     <t>Composer</t>
   </si>
   <si>
-    <t>On the Move!</t>
+    <t>Judy</t>
   </si>
   <si>
-    <t>Kofi Ansah, Andrew Klippel, David Haddad</t>
+    <t>Robert Walter, Eddie Roberts</t>
   </si>
   <si>
-    <t>Genesis Owusu</t>
+    <t>WRD</t>
   </si>
   <si>
-    <t>The Other Black Dog</t>
+    <t>Sleep Depraved</t>
   </si>
   <si>
-    <t>Kofi Ansah, Andrew Klippel, Michael Di Francesco</t>
+    <t>Robert Walter</t>
   </si>
   <si>
-    <t>Centrefold</t>
+    <t>Chum City</t>
   </si>
   <si>
-    <t>Kofi Ansah, Andrew Klippel, Kieran John Callinan, Di Francesco, Julian Sudek</t>
+    <t>Bobby's Boogaloo</t>
   </si>
   <si>
-    <t>Waitin' on Ya</t>
+    <t>Poison Dart</t>
   </si>
   <si>
-    <t>Don't Need You</t>
+    <t>Red Sunset</t>
   </si>
   <si>
-    <t>Kofi Ansah, Andrew Klippel, Kieran John Callinan, Di Francesco, Julian Sudek, David Haddad</t>
+    <t>Adam Deitch</t>
   </si>
   <si>
-    <t>Drown</t>
+    <t>Meditation</t>
   </si>
   <si>
-    <t>Genesis Owusu feat. Kirin J. Callinan</t>
+    <t>Samuel Henry Jr.</t>
   </si>
   <si>
-    <t>Gold Chains</t>
+    <t>Happy Hour</t>
   </si>
   <si>
-    <t>Smiling With No Teeth</t>
+    <t>Hot Honey</t>
   </si>
   <si>
-    <t>I Don't See Colour</t>
+    <t>Corner Pocket</t>
   </si>
   <si>
-    <t>Black Dogs!</t>
-  </si>
-  <si>
-    <t>Kofi Ansah, Matt Corby</t>
-  </si>
-  <si>
-    <t>Whip Cracker</t>
-  </si>
-  <si>
-    <t>Easy</t>
-  </si>
-  <si>
-    <t>Kofi Ansah, Harvey Sutherland</t>
-  </si>
-  <si>
-    <t>A Song About Fishing</t>
-  </si>
-  <si>
-    <t>No Looking Back</t>
-  </si>
-  <si>
-    <t>Bye Bye</t>
+    <t>Pump Up The Valium</t>
   </si>
 </sst>
 </file>
@@ -236,11 +215,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="genesisowusu1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="wrd1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="genesisowusu1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="wrd1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -549,10 +528,10 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.77734375" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="27.21875" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
@@ -588,7 +567,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>7.4305555555555555E-2</v>
+        <v>0.18472222222222223</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -609,7 +588,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>0.18263888888888891</v>
+        <v>0.17847222222222223</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -624,13 +603,13 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.1361111111111111</v>
+        <v>0.1875</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -642,16 +621,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>0.2388888888888889</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -663,16 +642,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>0.12847222222222224</v>
+        <v>0.21875</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -684,16 +663,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>0.12291666666666667</v>
+        <v>0.19166666666666665</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -705,16 +684,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="2">
-        <v>0.15138888888888888</v>
+        <v>0.14027777777777778</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -726,16 +705,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.2076388888888889</v>
+        <v>7.2222222222222229E-2</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -747,16 +726,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>0.12222222222222223</v>
+        <v>0.15</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -768,16 +747,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.12361111111111112</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -789,16 +768,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="2">
-        <v>0.19513888888888889</v>
+        <v>0.19027777777777777</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -806,84 +785,30 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.12638888888888888</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.1423611111111111</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.15416666666666667</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.17291666666666669</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -983,7 +908,7 @@
   <dimension ref="A2:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="A3:K19"/>
+      <selection activeCell="K15" sqref="A3:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -1003,15 +928,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -1031,21 +956,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                </v>
+        <v xml:space="preserve"> Title             </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                </v>
+        <v xml:space="preserve"> Composers                  </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                            </v>
+        <v xml:space="preserve"> Performer</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1070,21 +995,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">--------------------- </v>
+        <v xml:space="preserve">------------------ </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------------------------------------------------------ </v>
+        <v xml:space="preserve"> ---------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------- </v>
+        <v xml:space="preserve"> --------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1109,28 +1034,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">On the Move!         </v>
+        <v xml:space="preserve">Judy              </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Andrew Klippel, David Haddad                                                  </v>
+        <v xml:space="preserve"> Robert Walter, Eddie Roberts</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">WRD      </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:47 </v>
+        <v xml:space="preserve">04:26 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1149,28 +1074,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">The Other Black Dog  </v>
+        <v xml:space="preserve">Sleep Depraved    </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Andrew Klippel, Michael Di Francesco                                          </v>
+        <v xml:space="preserve"> Robert Walter               </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">WRD      </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:23 </v>
+        <v xml:space="preserve">04:17 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1189,28 +1114,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Centrefold           </v>
+        <v xml:space="preserve">Chum City         </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Andrew Klippel, Kieran John Callinan, Di Francesco, Julian Sudek              </v>
+        <v xml:space="preserve"> Robert Walter, Eddie Roberts</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">WRD      </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:16 </v>
+        <v xml:space="preserve">04:30 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1229,28 +1154,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Waitin' on Ya        </v>
+        <v xml:space="preserve">Bobby's Boogaloo  </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Andrew Klippel, Kieran John Callinan, Di Francesco, Julian Sudek              </v>
+        <v xml:space="preserve"> Robert Walter               </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">WRD      </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:44 </v>
+        <v xml:space="preserve">03:17 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1269,28 +1194,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Don't Need You       </v>
+        <v xml:space="preserve">Poison Dart       </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Andrew Klippel, Kieran John Callinan, Di Francesco, Julian Sudek, David Haddad</v>
+        <v xml:space="preserve"> Robert Walter               </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">WRD      </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:05 </v>
+        <v xml:space="preserve">05:15 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1309,28 +1234,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Drown                </v>
+        <v xml:space="preserve">Red Sunset        </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Andrew Klippel, Kieran John Callinan, Di Francesco, Julian Sudek, David Haddad</v>
+        <v xml:space="preserve"> Adam Deitch                 </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Genesis Owusu feat. Kirin J. Callinan</v>
+        <v xml:space="preserve">WRD      </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:57 </v>
+        <v xml:space="preserve">04:36 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1349,28 +1274,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Gold Chains          </v>
+        <v xml:space="preserve">Meditation        </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Andrew Klippel, Kieran John Callinan, Di Francesco, Julian Sudek              </v>
+        <v xml:space="preserve"> Samuel Henry Jr.            </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">WRD      </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:38 </v>
+        <v xml:space="preserve">03:22 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1389,28 +1314,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Smiling With No Teeth</v>
+        <v xml:space="preserve">Happy Hour        </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Andrew Klippel, Kieran John Callinan, Di Francesco, Julian Sudek              </v>
+        <v xml:space="preserve"> Robert Walter               </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">WRD      </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:59 </v>
+        <v xml:space="preserve">01:44 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1429,28 +1354,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">I Don't See Colour   </v>
+        <v xml:space="preserve">Hot Honey         </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Andrew Klippel, Kieran John Callinan, Di Francesco, Julian Sudek              </v>
+        <v xml:space="preserve"> Robert Walter               </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">WRD      </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:56 </v>
+        <v xml:space="preserve">03:36 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1469,28 +1394,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Black Dogs!          </v>
+        <v xml:space="preserve">Corner Pocket     </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Matt Corby                                                                    </v>
+        <v xml:space="preserve"> Adam Deitch                 </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">WRD      </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:00 </v>
+        <v xml:space="preserve">02:58 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1509,28 +1434,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Whip Cracker         </v>
+        <v>Pump Up The Valium</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Andrew Klippel, Kieran John Callinan, Di Francesco, Julian Sudek              </v>
+        <v xml:space="preserve"> Robert Walter               </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">WRD      </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:41 </v>
+        <v xml:space="preserve">04:34 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1542,35 +1467,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Easy                 </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Harvey Sutherland                                                             </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:02 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1582,35 +1507,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">A Song About Fishing </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Andrew Klippel, Kieran John Callinan, Di Francesco, Julian Sudek              </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:25 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1622,35 +1547,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">No Looking Back      </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Andrew Klippel, Kieran John Callinan, Di Francesco, Julian Sudek              </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:42 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1662,35 +1587,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Bye Bye              </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kofi Ansah, Andrew Klippel, Kieran John Callinan, Di Francesco, Julian Sudek              </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Genesis Owusu                        </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:09 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1709,21 +1634,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                           </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1749,21 +1674,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                           </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1789,21 +1714,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                           </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1829,21 +1754,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                           </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1869,21 +1794,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                           </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1909,21 +1834,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                           </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1949,21 +1874,21 @@
       </c>
       <c r="D26" t="str">
         <f>LEFTB(Sheet1!B23&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="str">
         <f>" "&amp;LEFTB(Sheet1!C23&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                           </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="G26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H26" t="str">
         <f>LEFTB(Sheet1!D23&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I26" s="4" t="s">
         <v>0</v>
@@ -1989,21 +1914,21 @@
       </c>
       <c r="D27" t="str">
         <f>LEFTB(Sheet1!B24&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="str">
         <f>" "&amp;LEFTB(Sheet1!C24&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                           </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="G27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H27" t="str">
         <f>LEFTB(Sheet1!D24&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I27" s="4" t="s">
         <v>0</v>
@@ -2034,10 +1959,10 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.77734375" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="27.21875" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
@@ -2073,7 +1998,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>7.4305555555555555E-2</v>
+        <v>0.18472222222222223</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2094,7 +2019,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>0.18263888888888891</v>
+        <v>0.17847222222222223</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2109,13 +2034,13 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.1361111111111111</v>
+        <v>0.1875</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2127,16 +2052,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>0.2388888888888889</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2148,16 +2073,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>0.12847222222222224</v>
+        <v>0.21875</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2169,16 +2094,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>0.12291666666666667</v>
+        <v>0.19166666666666665</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2190,16 +2115,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="2">
-        <v>0.15138888888888888</v>
+        <v>0.14027777777777778</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2211,16 +2136,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.2076388888888889</v>
+        <v>7.2222222222222229E-2</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2232,16 +2157,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>0.12222222222222223</v>
+        <v>0.15</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2253,16 +2178,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.12361111111111112</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2274,16 +2199,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="2">
-        <v>0.19513888888888889</v>
+        <v>0.19027777777777777</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2291,84 +2216,30 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.12638888888888888</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.1423611111111111</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.15416666666666667</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.17291666666666669</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>

</xml_diff>

<commit_message>
09292255 added review gp
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="wrd1_" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
-    <definedName name="wrd1_" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
+    <definedName name="greenteapeng1" localSheetId="0">Sheet1!$A$1:$E$19</definedName>
+    <definedName name="greenteapeng1" localSheetId="2">Sheet3!$A$1:$E$19</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/wrd1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/greenteapeng1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/wrd1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/greenteapeng1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="43">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -75,52 +75,112 @@
     <t>Composer</t>
   </si>
   <si>
-    <t>Judy</t>
-  </si>
-  <si>
-    <t>Robert Walter, Eddie Roberts</t>
-  </si>
-  <si>
-    <t>WRD</t>
-  </si>
-  <si>
-    <t>Sleep Depraved</t>
-  </si>
-  <si>
-    <t>Robert Walter</t>
-  </si>
-  <si>
-    <t>Chum City</t>
-  </si>
-  <si>
-    <t>Bobby's Boogaloo</t>
-  </si>
-  <si>
-    <t>Poison Dart</t>
-  </si>
-  <si>
-    <t>Red Sunset</t>
-  </si>
-  <si>
-    <t>Adam Deitch</t>
-  </si>
-  <si>
     <t>Meditation</t>
   </si>
   <si>
-    <t>Samuel Henry Jr.</t>
-  </si>
-  <si>
-    <t>Happy Hour</t>
-  </si>
-  <si>
-    <t>Hot Honey</t>
-  </si>
-  <si>
-    <t>Corner Pocket</t>
-  </si>
-  <si>
-    <t>Pump Up The Valium</t>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Make Noise</t>
+  </si>
+  <si>
+    <t>Aria Wells, Jake Harvey Tavemer, Joshua Kikonyogo, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones, Tom Hammond</t>
+  </si>
+  <si>
+    <t>Greentea Peng</t>
+  </si>
+  <si>
+    <t>This Sound</t>
+  </si>
+  <si>
+    <t>Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Mathew Anthony Kwasniewski-Kelvin, Richarf Crawford</t>
+  </si>
+  <si>
+    <t>Free My People</t>
+  </si>
+  <si>
+    <t>Aria Wells, George Joannides, Samuel Ampiah, Cameron Mathew Tomon, Anish Bhatt, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones,</t>
+  </si>
+  <si>
+    <t>Greentea Peng feat. Simmy, Kid Cruise</t>
+  </si>
+  <si>
+    <t>Be Careful</t>
+  </si>
+  <si>
+    <t>Aria Wells, Cameron Palmer, Tagara Mhiza, Jaega Francis McKenna-Gordon</t>
+  </si>
+  <si>
+    <t>Nah It Ain't the Same</t>
+  </si>
+  <si>
+    <t>Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones</t>
+  </si>
+  <si>
+    <t>Earnest</t>
+  </si>
+  <si>
+    <t>Aria Wells, Samo Castillano, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones, Tom Hamond</t>
+  </si>
+  <si>
+    <t>Suffer</t>
+  </si>
+  <si>
+    <t>Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield</t>
+  </si>
+  <si>
+    <t>Mataji Freestyle</t>
+  </si>
+  <si>
+    <t>Aria Wells, Anish Bhatt, Tagara Mhiza, Jaega Francis McKenna-Gordon, Joe Armon-Jones</t>
+  </si>
+  <si>
+    <t>Kali v2</t>
+  </si>
+  <si>
+    <t>Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Joe Armon-Jones</t>
+  </si>
+  <si>
+    <t>Satta</t>
+  </si>
+  <si>
+    <t>Aria Wells, Gordon Williams, Winston Riley</t>
+  </si>
+  <si>
+    <t>Party Hard (Interlude)</t>
+  </si>
+  <si>
+    <t>Aria Wells, Ian Greenidge, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones</t>
+  </si>
+  <si>
+    <t>Dingaling</t>
+  </si>
+  <si>
+    <t>Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Tony Olabode, Ryan Benton Thomas, Armedu uUgusutine, Idibia Innocent Ujah</t>
+  </si>
+  <si>
+    <t>Maya</t>
+  </si>
+  <si>
+    <t>Man Made</t>
+  </si>
+  <si>
+    <t>Aria Wells, Mark Lawrence, Tagara Mhiza, Jaega Francis McKenna-Gordon, Joe Armon-Jones</t>
+  </si>
+  <si>
+    <t>Poor Man (Skit)</t>
+  </si>
+  <si>
+    <t>Sinner</t>
+  </si>
+  <si>
+    <t>Aria Wells, Joshua Kikonyogo, Samo Castillano, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon</t>
+  </si>
+  <si>
+    <t>Jimtastic Blues</t>
+  </si>
+  <si>
+    <t>Aria Wells, Cameron Palmer, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon</t>
   </si>
 </sst>
 </file>
@@ -215,11 +275,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="wrd1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="greenteapeng1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="wrd1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="greenteapeng1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,11 +587,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="36.21875" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
@@ -540,6 +600,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -558,16 +621,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2">
-        <v>0.18472222222222223</v>
+        <v>0.14722222222222223</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -579,16 +642,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.17847222222222223</v>
+        <v>9.7916666666666666E-2</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -600,16 +663,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2">
-        <v>0.1875</v>
+        <v>0.14930555555555555</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -621,16 +684,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2">
-        <v>0.13680555555555554</v>
+        <v>0.1013888888888889</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -642,16 +705,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2">
-        <v>0.21875</v>
+        <v>0.17013888888888887</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -663,16 +726,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2">
-        <v>0.19166666666666665</v>
+        <v>0.15694444444444444</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -684,16 +747,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2">
-        <v>0.14027777777777778</v>
+        <v>0.12152777777777778</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -705,16 +768,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2">
-        <v>7.2222222222222229E-2</v>
+        <v>0.14722222222222223</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -726,16 +789,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2">
-        <v>0.15</v>
+        <v>0.12569444444444444</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -747,13 +810,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2">
         <v>0.12361111111111112</v>
@@ -768,16 +831,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2">
-        <v>0.19027777777777777</v>
+        <v>0.11180555555555556</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -785,113 +848,209 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.1388888888888889</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.1451388888888889</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.15138888888888888</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="E16" s="2"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.29652777777777778</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="5:10">
-      <c r="E17" s="2"/>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.10972222222222222</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="5:10">
-      <c r="E18" s="2"/>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9.7222222222222224E-2</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="5:10">
-      <c r="E19" s="2"/>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.14930555555555555</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="5:10">
+    <row r="20" spans="1:10">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="5:10">
+    <row r="21" spans="1:10">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="5:10">
+    <row r="22" spans="1:10">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="5:10">
+    <row r="23" spans="1:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="5:10">
+    <row r="24" spans="1:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="5:10">
+    <row r="25" spans="1:10">
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="5:10">
+    <row r="26" spans="1:10">
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="5:10">
+    <row r="27" spans="1:10">
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="5:10">
+    <row r="28" spans="1:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="5:10">
+    <row r="29" spans="1:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="5:10">
+    <row r="30" spans="1:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="5:10">
+    <row r="31" spans="1:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="5:10">
+    <row r="32" spans="1:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">
@@ -908,7 +1067,7 @@
   <dimension ref="A2:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="A3:K15"/>
+      <selection activeCell="K22" sqref="A3:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -928,15 +1087,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>28</v>
+        <v>162</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -956,21 +1115,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title             </v>
+        <v xml:space="preserve"> Title                 </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                  </v>
+        <v xml:space="preserve"> Composers                                                                                                                                                        </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer</v>
+        <v xml:space="preserve"> Performer                            </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -995,21 +1154,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------ </v>
+        <v xml:space="preserve">---------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------------------------------------------------ </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> --------- </v>
+        <v xml:space="preserve"> ------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1034,28 +1193,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Judy              </v>
+        <v xml:space="preserve">Make Noise            </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Robert Walter, Eddie Roberts</v>
+        <v xml:space="preserve"> Aria Wells, Jake Harvey Tavemer, Joshua Kikonyogo, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones, Tom Hammond</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">WRD      </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:26 </v>
+        <v xml:space="preserve">03:32 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1074,28 +1233,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sleep Depraved    </v>
+        <v xml:space="preserve">This Sound            </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Robert Walter               </v>
+        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Mathew Anthony Kwasniewski-Kelvin, Richarf Crawford                </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">WRD      </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:17 </v>
+        <v xml:space="preserve">02:21 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1114,28 +1273,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Chum City         </v>
+        <v xml:space="preserve">Free My People        </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Robert Walter, Eddie Roberts</v>
+        <v xml:space="preserve"> Aria Wells, George Joannides, Samuel Ampiah, Cameron Mathew Tomon, Anish Bhatt, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones,          </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">WRD      </v>
+        <v>Greentea Peng feat. Simmy, Kid Cruise</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:30 </v>
+        <v xml:space="preserve">03:35 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1154,28 +1313,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Bobby's Boogaloo  </v>
+        <v xml:space="preserve">Be Careful            </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Robert Walter               </v>
+        <v xml:space="preserve"> Aria Wells, Cameron Palmer, Tagara Mhiza, Jaega Francis McKenna-Gordon                                                                                            </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">WRD      </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:17 </v>
+        <v xml:space="preserve">02:26 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1194,28 +1353,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Poison Dart       </v>
+        <v xml:space="preserve">Nah It Ain't the Same </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Robert Walter               </v>
+        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones                                                    </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">WRD      </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:15 </v>
+        <v xml:space="preserve">04:05 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1234,28 +1393,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Red Sunset        </v>
+        <v xml:space="preserve">Earnest               </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Adam Deitch                 </v>
+        <v xml:space="preserve"> Aria Wells, Samo Castillano, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones, Tom Hamond                       </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">WRD      </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:36 </v>
+        <v xml:space="preserve">03:46 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1274,28 +1433,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Meditation        </v>
+        <v xml:space="preserve">Suffer                </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Samuel Henry Jr.            </v>
+        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield                                                                                                   </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">WRD      </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:22 </v>
+        <v xml:space="preserve">02:55 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1314,28 +1473,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Happy Hour        </v>
+        <v xml:space="preserve">Mataji Freestyle      </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Robert Walter               </v>
+        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jaega Francis McKenna-Gordon, Joe Armon-Jones                                                                              </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">WRD      </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:44 </v>
+        <v xml:space="preserve">03:32 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1354,28 +1513,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Hot Honey         </v>
+        <v xml:space="preserve">Kali v2               </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Robert Walter               </v>
+        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Joe Armon-Jones                                                                                  </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">WRD      </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:36 </v>
+        <v xml:space="preserve">03:01 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1394,21 +1553,21 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Corner Pocket     </v>
+        <v xml:space="preserve">Satta                 </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Adam Deitch                 </v>
+        <v xml:space="preserve"> Aria Wells, Gordon Williams, Winston Riley                                                                                                                        </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">WRD      </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
@@ -1434,28 +1593,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Pump Up The Valium</v>
+        <v>Party Hard (Interlude)</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Robert Walter               </v>
+        <v xml:space="preserve"> Aria Wells, Ian Greenidge, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones                                     </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">WRD      </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:34 </v>
+        <v xml:space="preserve">02:41 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1467,35 +1626,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Dingaling             </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Tony Olabode, Ryan Benton Thomas, Armedu uUgusutine, Idibia Innocent Ujah                        </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:20 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1507,35 +1666,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Maya                  </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield                                                                                                   </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:29 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1547,35 +1706,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Man Made              </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve"> Aria Wells, Mark Lawrence, Tagara Mhiza, Jaega Francis McKenna-Gordon, Joe Armon-Jones                                                                            </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:38 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1587,35 +1746,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Meditation            </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones                                                    </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">07:07 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1627,35 +1786,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Poor Man (Skit)       </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jaega Francis McKenna-Gordon, Joe Armon-Jones                                                                              </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:38 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1667,35 +1826,35 @@
       </c>
       <c r="B21">
         <f>Sheet1!A18</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Sinner                </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve"> Aria Wells, Joshua Kikonyogo, Samo Castillano, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon                                               </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:20 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
@@ -1707,35 +1866,35 @@
       </c>
       <c r="B22">
         <f>Sheet1!A19</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Jimtastic Blues       </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve"> Aria Wells, Cameron Palmer, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon                                                                  </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">Greentea Peng                        </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="3" t="str">
         <f>TEXT(Sheet1!E19,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:35 </v>
       </c>
       <c r="K22" s="4" t="s">
         <v>0</v>
@@ -1754,21 +1913,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve">                                                                                                                                                                   </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1794,21 +1953,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve">                                                                                                                                                                   </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1834,21 +1993,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve">                                                                                                                                                                   </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1874,21 +2033,21 @@
       </c>
       <c r="D26" t="str">
         <f>LEFTB(Sheet1!B23&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="str">
         <f>" "&amp;LEFTB(Sheet1!C23&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve">                                                                                                                                                                   </v>
       </c>
       <c r="G26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H26" t="str">
         <f>LEFTB(Sheet1!D23&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I26" s="4" t="s">
         <v>0</v>
@@ -1914,21 +2073,21 @@
       </c>
       <c r="D27" t="str">
         <f>LEFTB(Sheet1!B24&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="str">
         <f>" "&amp;LEFTB(Sheet1!C24&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve">                                                                                                                                                                   </v>
       </c>
       <c r="G27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H27" t="str">
         <f>LEFTB(Sheet1!D24&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I27" s="4" t="s">
         <v>0</v>
@@ -1953,16 +2112,16 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="36.21875" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
@@ -1971,6 +2130,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -1989,16 +2151,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2">
-        <v>0.18472222222222223</v>
+        <v>0.14722222222222223</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2010,16 +2172,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.17847222222222223</v>
+        <v>9.7916666666666666E-2</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2031,16 +2193,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2">
-        <v>0.1875</v>
+        <v>0.14930555555555555</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2052,16 +2214,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2">
-        <v>0.13680555555555554</v>
+        <v>0.1013888888888889</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2073,16 +2235,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2">
-        <v>0.21875</v>
+        <v>0.17013888888888887</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2094,16 +2256,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2">
-        <v>0.19166666666666665</v>
+        <v>0.15694444444444444</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2115,16 +2277,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2">
-        <v>0.14027777777777778</v>
+        <v>0.12152777777777778</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2136,16 +2298,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2">
-        <v>7.2222222222222229E-2</v>
+        <v>0.14722222222222223</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2157,16 +2319,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2">
-        <v>0.15</v>
+        <v>0.12569444444444444</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2178,13 +2340,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2">
         <v>0.12361111111111112</v>
@@ -2199,16 +2361,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2">
-        <v>0.19027777777777777</v>
+        <v>0.11180555555555556</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2216,113 +2378,209 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.1388888888888889</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.1451388888888889</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.15138888888888888</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="E16" s="2"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.29652777777777778</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="5:10">
-      <c r="E17" s="2"/>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.10972222222222222</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="5:10">
-      <c r="E18" s="2"/>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9.7222222222222224E-2</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="5:10">
-      <c r="E19" s="2"/>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.14930555555555555</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="5:10">
+    <row r="20" spans="1:10">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="5:10">
+    <row r="21" spans="1:10">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="5:10">
+    <row r="22" spans="1:10">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="5:10">
+    <row r="23" spans="1:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="5:10">
+    <row r="24" spans="1:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="5:10">
+    <row r="25" spans="1:10">
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="5:10">
+    <row r="26" spans="1:10">
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="5:10">
+    <row r="27" spans="1:10">
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="5:10">
+    <row r="28" spans="1:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="5:10">
+    <row r="29" spans="1:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="5:10">
+    <row r="30" spans="1:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="5:10">
+    <row r="31" spans="1:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="5:10">
+    <row r="32" spans="1:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">

</xml_diff>

<commit_message>
11122245 added review st jc
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="greenteapeng1" localSheetId="0">Sheet1!$A$1:$E$19</definedName>
-    <definedName name="greenteapeng1" localSheetId="2">Sheet3!$A$1:$E$19</definedName>
+    <definedName name="jcole4" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
+    <definedName name="jcole4" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/greenteapeng1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/jcole4.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/greenteapeng1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/jcole4.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="29">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -75,112 +75,70 @@
     <t>Composer</t>
   </si>
   <si>
-    <t>Meditation</t>
-  </si>
-  <si>
     <t>No.</t>
   </si>
   <si>
-    <t>Make Noise</t>
-  </si>
-  <si>
-    <t>Aria Wells, Jake Harvey Tavemer, Joshua Kikonyogo, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones, Tom Hammond</t>
-  </si>
-  <si>
-    <t>Greentea Peng</t>
-  </si>
-  <si>
-    <t>This Sound</t>
-  </si>
-  <si>
-    <t>Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Mathew Anthony Kwasniewski-Kelvin, Richarf Crawford</t>
-  </si>
-  <si>
-    <t>Free My People</t>
-  </si>
-  <si>
-    <t>Aria Wells, George Joannides, Samuel Ampiah, Cameron Mathew Tomon, Anish Bhatt, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones,</t>
-  </si>
-  <si>
-    <t>Greentea Peng feat. Simmy, Kid Cruise</t>
-  </si>
-  <si>
-    <t>Be Careful</t>
-  </si>
-  <si>
-    <t>Aria Wells, Cameron Palmer, Tagara Mhiza, Jaega Francis McKenna-Gordon</t>
-  </si>
-  <si>
-    <t>Nah It Ain't the Same</t>
-  </si>
-  <si>
-    <t>Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones</t>
-  </si>
-  <si>
-    <t>Earnest</t>
-  </si>
-  <si>
-    <t>Aria Wells, Samo Castillano, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones, Tom Hamond</t>
-  </si>
-  <si>
-    <t>Suffer</t>
-  </si>
-  <si>
-    <t>Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield</t>
-  </si>
-  <si>
-    <t>Mataji Freestyle</t>
-  </si>
-  <si>
-    <t>Aria Wells, Anish Bhatt, Tagara Mhiza, Jaega Francis McKenna-Gordon, Joe Armon-Jones</t>
-  </si>
-  <si>
-    <t>Kali v2</t>
-  </si>
-  <si>
-    <t>Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Joe Armon-Jones</t>
-  </si>
-  <si>
-    <t>Satta</t>
-  </si>
-  <si>
-    <t>Aria Wells, Gordon Williams, Winston Riley</t>
-  </si>
-  <si>
-    <t>Party Hard (Interlude)</t>
-  </si>
-  <si>
-    <t>Aria Wells, Ian Greenidge, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones</t>
-  </si>
-  <si>
-    <t>Dingaling</t>
-  </si>
-  <si>
-    <t>Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Tony Olabode, Ryan Benton Thomas, Armedu uUgusutine, Idibia Innocent Ujah</t>
-  </si>
-  <si>
-    <t>Maya</t>
-  </si>
-  <si>
-    <t>Man Made</t>
-  </si>
-  <si>
-    <t>Aria Wells, Mark Lawrence, Tagara Mhiza, Jaega Francis McKenna-Gordon, Joe Armon-Jones</t>
-  </si>
-  <si>
-    <t>Poor Man (Skit)</t>
-  </si>
-  <si>
-    <t>Sinner</t>
-  </si>
-  <si>
-    <t>Aria Wells, Joshua Kikonyogo, Samo Castillano, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon</t>
-  </si>
-  <si>
-    <t>Jimtastic Blues</t>
-  </si>
-  <si>
-    <t>Aria Wells, Cameron Palmer, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon</t>
+    <t>9 5 . s o u t h</t>
+  </si>
+  <si>
+    <t>J. Cole</t>
+  </si>
+  <si>
+    <t>a m a r i</t>
+  </si>
+  <si>
+    <t>m y . l i f e</t>
+  </si>
+  <si>
+    <t>J. Cole / 21 Savage</t>
+  </si>
+  <si>
+    <t>J. Cole feat: Morray / 21 Savage</t>
+  </si>
+  <si>
+    <t>a p p l y i n g . p r e s s u r e</t>
+  </si>
+  <si>
+    <t>p u n c h i n ‘ . t h e . c l o c k</t>
+  </si>
+  <si>
+    <t>1 0 0 . m i l ‘</t>
+  </si>
+  <si>
+    <t>J. Cole feat: Bas</t>
+  </si>
+  <si>
+    <t>p r i d e . i s . t h e . d e v i l</t>
+  </si>
+  <si>
+    <t>Lil Baby / J. Cole</t>
+  </si>
+  <si>
+    <t>J. Cole feat: Lil Baby</t>
+  </si>
+  <si>
+    <t>l e t . g o . m y . h a n d</t>
+  </si>
+  <si>
+    <t>Bas / J. Cole</t>
+  </si>
+  <si>
+    <t>J. Cole feat: 6LACK / Bas</t>
+  </si>
+  <si>
+    <t>i n t e r l u d e</t>
+  </si>
+  <si>
+    <t>The c l i m b . b a c k</t>
+  </si>
+  <si>
+    <t>Maximilian Axelrod / Gary Bailey / Montey Bailey / J. Cole</t>
+  </si>
+  <si>
+    <t>c l o s e</t>
+  </si>
+  <si>
+    <t>h u n g e r . o n . h i l l s i d e</t>
   </si>
 </sst>
 </file>
@@ -275,11 +233,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="greenteapeng1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jcole4" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="greenteapeng1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jcole4" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -588,9 +546,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="36.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="3" max="3" width="53.5546875" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
@@ -601,7 +559,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -621,16 +579,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.14722222222222223</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -642,16 +600,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>9.7916666666666666E-2</v>
+        <v>0.10277777777777779</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -663,16 +621,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
-        <v>0.14930555555555555</v>
+        <v>0.15208333333333332</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -684,16 +642,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>0.1013888888888889</v>
+        <v>0.12291666666666667</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -705,16 +663,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>0.17013888888888887</v>
+        <v>7.7777777777777779E-2</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -726,16 +684,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2">
-        <v>0.15694444444444444</v>
+        <v>0.11319444444444444</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -747,16 +705,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2">
-        <v>0.12152777777777778</v>
+        <v>0.15138888888888888</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -768,16 +726,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2">
-        <v>0.14722222222222223</v>
+        <v>0.18472222222222223</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -789,16 +747,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>0.12569444444444444</v>
+        <v>9.0972222222222218E-2</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -810,16 +768,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>0.12361111111111112</v>
+        <v>0.21180555555555555</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -831,16 +789,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2">
-        <v>0.11180555555555556</v>
+        <v>0.1173611111111111</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -852,16 +810,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E13" s="5">
-        <v>0.1388888888888889</v>
+        <v>0.16597222222222222</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
@@ -869,188 +827,104 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.1451388888888889</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.15138888888888888</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.29652777777777778</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.10972222222222222</v>
-      </c>
+    <row r="17" spans="5:10">
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="2">
-        <v>9.7222222222222224E-2</v>
-      </c>
+    <row r="18" spans="5:10">
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.14930555555555555</v>
-      </c>
+    <row r="19" spans="5:10">
+      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="5:10">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="5:10">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="5:10">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="5:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="5:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="5:10">
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="5:10">
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="5:10">
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="5:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="5:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="5:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="5:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="5:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">
@@ -1067,7 +941,7 @@
   <dimension ref="A2:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="A3:K22"/>
+      <selection activeCell="K16" sqref="A3:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -1087,15 +961,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>162</v>
+        <v>58</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -1115,21 +989,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                 </v>
+        <v xml:space="preserve"> Title                               </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                                        </v>
+        <v xml:space="preserve"> Composers                                                </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                            </v>
+        <v xml:space="preserve"> Performer                       </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1154,21 +1028,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">---------------------- </v>
+        <v xml:space="preserve">------------------------------------ </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------------------------------------------------ </v>
+        <v xml:space="preserve"> ---------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------- </v>
+        <v xml:space="preserve"> -------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1193,28 +1067,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Make Noise            </v>
+        <v xml:space="preserve">9 5 . s o u t h                     </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Jake Harvey Tavemer, Joshua Kikonyogo, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones, Tom Hammond</v>
+        <v xml:space="preserve"> J. Cole                                                   </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">J. Cole                         </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:32 </v>
+        <v xml:space="preserve">03:17 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1233,28 +1107,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">This Sound            </v>
+        <v xml:space="preserve">a m a r i                           </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Mathew Anthony Kwasniewski-Kelvin, Richarf Crawford                </v>
+        <v xml:space="preserve"> J. Cole                                                   </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">J. Cole                         </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:21 </v>
+        <v xml:space="preserve">02:28 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1273,28 +1147,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Free My People        </v>
+        <v xml:space="preserve">m y . l i f e                       </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, George Joannides, Samuel Ampiah, Cameron Mathew Tomon, Anish Bhatt, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones,          </v>
+        <v xml:space="preserve"> J. Cole / 21 Savage                                       </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Greentea Peng feat. Simmy, Kid Cruise</v>
+        <v>J. Cole feat: Morray / 21 Savage</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:35 </v>
+        <v xml:space="preserve">03:39 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1313,28 +1187,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Be Careful            </v>
+        <v xml:space="preserve">a p p l y i n g . p r e s s u r e   </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Cameron Palmer, Tagara Mhiza, Jaega Francis McKenna-Gordon                                                                                            </v>
+        <v xml:space="preserve"> J. Cole                                                   </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">J. Cole                         </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:26 </v>
+        <v xml:space="preserve">02:57 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1353,28 +1227,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Nah It Ain't the Same </v>
+        <v>p u n c h i n ‘ . t h e . c l o c k</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones                                                    </v>
+        <v xml:space="preserve"> J. Cole                                                   </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">J. Cole                         </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:05 </v>
+        <v xml:space="preserve">01:52 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1393,28 +1267,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Earnest               </v>
+        <v xml:space="preserve">1 0 0 . m i l ‘                    </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Samo Castillano, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones, Tom Hamond                       </v>
+        <v xml:space="preserve"> J. Cole                                                   </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">J. Cole feat: Bas               </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:46 </v>
+        <v xml:space="preserve">02:43 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1433,28 +1307,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Suffer                </v>
+        <v xml:space="preserve">p r i d e . i s . t h e . d e v i l </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield                                                                                                   </v>
+        <v xml:space="preserve"> Lil Baby / J. Cole                                        </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">J. Cole feat: Lil Baby          </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:55 </v>
+        <v xml:space="preserve">03:38 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1473,28 +1347,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Mataji Freestyle      </v>
+        <v xml:space="preserve">l e t . g o . m y . h a n d         </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jaega Francis McKenna-Gordon, Joe Armon-Jones                                                                              </v>
+        <v xml:space="preserve"> Bas / J. Cole                                             </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">J. Cole feat: 6LACK / Bas       </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:32 </v>
+        <v xml:space="preserve">04:26 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1513,28 +1387,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Kali v2               </v>
+        <v xml:space="preserve">i n t e r l u d e                   </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Joe Armon-Jones                                                                                  </v>
+        <v xml:space="preserve"> J. Cole                                                   </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">J. Cole                         </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:01 </v>
+        <v xml:space="preserve">02:11 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1553,28 +1427,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Satta                 </v>
+        <v xml:space="preserve">The c l i m b . b a c k             </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Gordon Williams, Winston Riley                                                                                                                        </v>
+        <v xml:space="preserve"> Maximilian Axelrod / Gary Bailey / Montey Bailey / J. Cole</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">J. Cole                         </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:58 </v>
+        <v xml:space="preserve">05:05 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1593,28 +1467,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Party Hard (Interlude)</v>
+        <v xml:space="preserve">c l o s e                           </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Ian Greenidge, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones                                     </v>
+        <v xml:space="preserve"> J. Cole                                                   </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">J. Cole                         </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:41 </v>
+        <v xml:space="preserve">02:49 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1633,28 +1507,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Dingaling             </v>
+        <v xml:space="preserve">h u n g e r . o n . h i l l s i d e </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Tony Olabode, Ryan Benton Thomas, Armedu uUgusutine, Idibia Innocent Ujah                        </v>
+        <v xml:space="preserve"> J. Cole                                                   </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">J. Cole feat: Bas               </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:20 </v>
+        <v xml:space="preserve">03:59 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1666,35 +1540,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Maya                  </v>
+        <v xml:space="preserve">                                    </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield                                                                                                   </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:29 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1706,35 +1580,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Man Made              </v>
+        <v xml:space="preserve">                                    </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Mark Lawrence, Tagara Mhiza, Jaega Francis McKenna-Gordon, Joe Armon-Jones                                                                            </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:38 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1746,35 +1620,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Meditation            </v>
+        <v xml:space="preserve">                                    </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon, Joe Armon-Jones                                                    </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">07:07 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1786,35 +1660,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Poor Man (Skit)       </v>
+        <v xml:space="preserve">                                    </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Anish Bhatt, Tagara Mhiza, Jaega Francis McKenna-Gordon, Joe Armon-Jones                                                                              </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:38 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1826,35 +1700,35 @@
       </c>
       <c r="B21">
         <f>Sheet1!A18</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sinner                </v>
+        <v xml:space="preserve">                                    </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Joshua Kikonyogo, Samo Castillano, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon                                               </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:20 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
@@ -1866,35 +1740,35 @@
       </c>
       <c r="B22">
         <f>Sheet1!A19</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Jimtastic Blues       </v>
+        <v xml:space="preserve">                                    </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aria Wells, Cameron Palmer, Tagara Mhiza, Jordan Thompson Hadfield, Jaega Francis McKenna-Gordon                                                                  </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Greentea Peng                        </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="3" t="str">
         <f>TEXT(Sheet1!E19,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:35 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K22" s="4" t="s">
         <v>0</v>
@@ -1913,21 +1787,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                                    </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1953,21 +1827,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                                    </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1993,21 +1867,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                                    </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -2033,21 +1907,21 @@
       </c>
       <c r="D26" t="str">
         <f>LEFTB(Sheet1!B23&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                                    </v>
       </c>
       <c r="E26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="str">
         <f>" "&amp;LEFTB(Sheet1!C23&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H26" t="str">
         <f>LEFTB(Sheet1!D23&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="I26" s="4" t="s">
         <v>0</v>
@@ -2073,21 +1947,21 @@
       </c>
       <c r="D27" t="str">
         <f>LEFTB(Sheet1!B24&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                                    </v>
       </c>
       <c r="E27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="str">
         <f>" "&amp;LEFTB(Sheet1!C24&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H27" t="str">
         <f>LEFTB(Sheet1!D24&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="I27" s="4" t="s">
         <v>0</v>
@@ -2112,15 +1986,15 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="36.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="3" max="3" width="53.5546875" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
@@ -2131,7 +2005,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -2151,16 +2025,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.14722222222222223</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2172,16 +2046,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>9.7916666666666666E-2</v>
+        <v>0.10277777777777779</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2193,16 +2067,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
-        <v>0.14930555555555555</v>
+        <v>0.15208333333333332</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2214,16 +2088,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>0.1013888888888889</v>
+        <v>0.12291666666666667</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2235,16 +2109,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>0.17013888888888887</v>
+        <v>7.7777777777777779E-2</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2256,16 +2130,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2">
-        <v>0.15694444444444444</v>
+        <v>0.11319444444444444</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2277,16 +2151,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2">
-        <v>0.12152777777777778</v>
+        <v>0.15138888888888888</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2298,16 +2172,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2">
-        <v>0.14722222222222223</v>
+        <v>0.18472222222222223</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2319,16 +2193,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>0.12569444444444444</v>
+        <v>9.0972222222222218E-2</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2340,16 +2214,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>0.12361111111111112</v>
+        <v>0.21180555555555555</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2361,16 +2235,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2">
-        <v>0.11180555555555556</v>
+        <v>0.1173611111111111</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2382,16 +2256,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E13" s="5">
-        <v>0.1388888888888889</v>
+        <v>0.16597222222222222</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
@@ -2399,188 +2273,104 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.1451388888888889</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.15138888888888888</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.29652777777777778</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.10972222222222222</v>
-      </c>
+    <row r="17" spans="5:10">
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="2">
-        <v>9.7222222222222224E-2</v>
-      </c>
+    <row r="18" spans="5:10">
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.14930555555555555</v>
-      </c>
+    <row r="19" spans="5:10">
+      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="5:10">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="5:10">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="5:10">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="5:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="5:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="5:10">
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="5:10">
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="5:10">
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="5:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="5:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="5:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="5:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="5:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">

</xml_diff>

<commit_message>
10202315 added review lm
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="jcole4" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
-    <definedName name="jcole4" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
+    <definedName name="lauramvula3" localSheetId="0">Sheet1!$A$1:$E$11</definedName>
+    <definedName name="lauramvula3" localSheetId="2">Sheet3!$A$1:$E$11</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/jcole4.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/lauramvula3.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/jcole4.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/lauramvula3.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="20">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -75,70 +75,43 @@
     <t>Composer</t>
   </si>
   <si>
-    <t>No.</t>
+    <t>Safe Passage</t>
   </si>
   <si>
-    <t>9 5 . s o u t h</t>
+    <t>Laura Mvula, Dann Hume</t>
   </si>
   <si>
-    <t>J. Cole</t>
+    <t>Laura Mvula</t>
   </si>
   <si>
-    <t>a m a r i</t>
+    <t>Conditional</t>
   </si>
   <si>
-    <t>m y . l i f e</t>
+    <t>Church Girl</t>
   </si>
   <si>
-    <t>J. Cole / 21 Savage</t>
+    <t>Remedy</t>
   </si>
   <si>
-    <t>J. Cole feat: Morray / 21 Savage</t>
+    <t>Magical</t>
   </si>
   <si>
-    <t>a p p l y i n g . p r e s s u r e</t>
+    <t>Pink Noise</t>
   </si>
   <si>
-    <t>p u n c h i n ‘ . t h e . c l o c k</t>
+    <t>Golden Ashes</t>
   </si>
   <si>
-    <t>1 0 0 . m i l ‘</t>
+    <t>What Matters</t>
   </si>
   <si>
-    <t>J. Cole feat: Bas</t>
+    <t>Laura Mvul, Simon Neil</t>
   </si>
   <si>
-    <t>p r i d e . i s . t h e . d e v i l</t>
+    <t>Got Me</t>
   </si>
   <si>
-    <t>Lil Baby / J. Cole</t>
-  </si>
-  <si>
-    <t>J. Cole feat: Lil Baby</t>
-  </si>
-  <si>
-    <t>l e t . g o . m y . h a n d</t>
-  </si>
-  <si>
-    <t>Bas / J. Cole</t>
-  </si>
-  <si>
-    <t>J. Cole feat: 6LACK / Bas</t>
-  </si>
-  <si>
-    <t>i n t e r l u d e</t>
-  </si>
-  <si>
-    <t>The c l i m b . b a c k</t>
-  </si>
-  <si>
-    <t>Maximilian Axelrod / Gary Bailey / Montey Bailey / J. Cole</t>
-  </si>
-  <si>
-    <t>c l o s e</t>
-  </si>
-  <si>
-    <t>h u n g e r . o n . h i l l s i d e</t>
+    <t>Before the Dawn</t>
   </si>
 </sst>
 </file>
@@ -233,11 +206,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jcole4" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="lauramvula3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jcole4" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="lauramvula3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,11 +518,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" customWidth="1"/>
-    <col min="3" max="3" width="53.5546875" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
@@ -558,9 +531,6 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -579,16 +549,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.13680555555555554</v>
+        <v>0.13402777777777777</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -603,13 +573,13 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>0.10277777777777779</v>
+        <v>0.1173611111111111</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -624,13 +594,13 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15208333333333332</v>
+        <v>0.15625</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -642,16 +612,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>0.12291666666666667</v>
+        <v>0.16805555555555554</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -663,16 +633,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>7.7777777777777779E-2</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -684,16 +654,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
       <c r="E7" s="2">
-        <v>0.11319444444444444</v>
+        <v>0.1451388888888889</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -705,16 +675,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2">
-        <v>0.15138888888888888</v>
+        <v>0.17291666666666669</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -726,16 +696,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2">
-        <v>0.18472222222222223</v>
+        <v>0.17222222222222225</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -747,16 +717,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>9.0972222222222218E-2</v>
+        <v>0.14305555555555557</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -768,16 +738,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>0.21180555555555555</v>
+        <v>0.18194444444444444</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -785,42 +755,16 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.1173611111111111</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.16597222222222222</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -941,7 +885,7 @@
   <dimension ref="A2:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="A3:K16"/>
+      <selection activeCell="K14" sqref="A3:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -961,15 +905,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -989,21 +933,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                               </v>
+        <v xml:space="preserve"> Title          </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                </v>
+        <v xml:space="preserve"> Composers            </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                       </v>
+        <v xml:space="preserve"> Performer             </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1028,21 +972,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------------------------ </v>
+        <v xml:space="preserve">--------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------------------------------- </v>
+        <v xml:space="preserve"> ---------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> -------------------------------- </v>
+        <v xml:space="preserve"> ---------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1067,28 +1011,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">9 5 . s o u t h                     </v>
+        <v xml:space="preserve">Safe Passage   </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> J. Cole                                                   </v>
+        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                         </v>
+        <v xml:space="preserve">Laura Mvula           </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:17 </v>
+        <v xml:space="preserve">03:13 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1107,28 +1051,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">a m a r i                           </v>
+        <v xml:space="preserve">Conditional    </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> J. Cole                                                   </v>
+        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                         </v>
+        <v xml:space="preserve">Laura Mvula           </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:28 </v>
+        <v xml:space="preserve">02:49 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1147,28 +1091,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">m y . l i f e                       </v>
+        <v xml:space="preserve">Church Girl    </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> J. Cole / 21 Savage                                       </v>
+        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>J. Cole feat: Morray / 21 Savage</v>
+        <v xml:space="preserve">Laura Mvula           </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:39 </v>
+        <v xml:space="preserve">03:45 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1187,28 +1131,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">a p p l y i n g . p r e s s u r e   </v>
+        <v xml:space="preserve">Remedy         </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> J. Cole                                                   </v>
+        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                         </v>
+        <v xml:space="preserve">Laura Mvula           </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:57 </v>
+        <v xml:space="preserve">04:02 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1227,28 +1171,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>p u n c h i n ‘ . t h e . c l o c k</v>
+        <v xml:space="preserve">Magical        </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> J. Cole                                                   </v>
+        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                         </v>
+        <v xml:space="preserve">Laura Mvula           </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:52 </v>
+        <v xml:space="preserve">04:12 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1267,28 +1211,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">1 0 0 . m i l ‘                    </v>
+        <v xml:space="preserve">Pink Noise     </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> J. Cole                                                   </v>
+        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole feat: Bas               </v>
+        <v xml:space="preserve">Laura Mvula           </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:43 </v>
+        <v xml:space="preserve">03:29 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1307,28 +1251,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">p r i d e . i s . t h e . d e v i l </v>
+        <v xml:space="preserve">Golden Ashes   </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Lil Baby / J. Cole                                        </v>
+        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole feat: Lil Baby          </v>
+        <v xml:space="preserve">Laura Mvula           </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:38 </v>
+        <v xml:space="preserve">04:09 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1347,28 +1291,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">l e t . g o . m y . h a n d         </v>
+        <v xml:space="preserve">What Matters   </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Bas / J. Cole                                             </v>
+        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole feat: 6LACK / Bas       </v>
+        <v>Laura Mvul, Simon Neil</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:26 </v>
+        <v xml:space="preserve">04:08 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1387,28 +1331,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">i n t e r l u d e                   </v>
+        <v xml:space="preserve">Got Me         </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> J. Cole                                                   </v>
+        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                         </v>
+        <v xml:space="preserve">Laura Mvula           </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:11 </v>
+        <v xml:space="preserve">03:26 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1427,28 +1371,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">The c l i m b . b a c k             </v>
+        <v>Before the Dawn</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Maximilian Axelrod / Gary Bailey / Montey Bailey / J. Cole</v>
+        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                         </v>
+        <v xml:space="preserve">Laura Mvula           </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:05 </v>
+        <v xml:space="preserve">04:22 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1460,35 +1404,35 @@
       </c>
       <c r="B15">
         <f>Sheet1!A12</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">c l o s e                           </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> J. Cole                                                   </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                         </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:49 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1500,35 +1444,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">h u n g e r . o n . h i l l s i d e </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> J. Cole                                                   </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole feat: Bas               </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:59 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1547,21 +1491,21 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
@@ -1587,21 +1531,21 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
@@ -1627,21 +1571,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1667,21 +1611,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1707,21 +1651,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1747,21 +1691,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1787,21 +1731,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1827,21 +1771,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1867,21 +1811,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1907,21 +1851,21 @@
       </c>
       <c r="D26" t="str">
         <f>LEFTB(Sheet1!B23&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="str">
         <f>" "&amp;LEFTB(Sheet1!C23&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="G26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H26" t="str">
         <f>LEFTB(Sheet1!D23&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="I26" s="4" t="s">
         <v>0</v>
@@ -1947,21 +1891,21 @@
       </c>
       <c r="D27" t="str">
         <f>LEFTB(Sheet1!B24&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="str">
         <f>" "&amp;LEFTB(Sheet1!C24&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="G27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H27" t="str">
         <f>LEFTB(Sheet1!D24&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="I27" s="4" t="s">
         <v>0</v>
@@ -1991,11 +1935,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" customWidth="1"/>
-    <col min="3" max="3" width="53.5546875" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
@@ -2004,9 +1948,6 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -2025,16 +1966,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.13680555555555554</v>
+        <v>0.13402777777777777</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2049,13 +1990,13 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>0.10277777777777779</v>
+        <v>0.1173611111111111</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2070,13 +2011,13 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15208333333333332</v>
+        <v>0.15625</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2088,16 +2029,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>0.12291666666666667</v>
+        <v>0.16805555555555554</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2109,16 +2050,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>7.7777777777777779E-2</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2130,16 +2071,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
       <c r="E7" s="2">
-        <v>0.11319444444444444</v>
+        <v>0.1451388888888889</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2151,16 +2092,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2">
-        <v>0.15138888888888888</v>
+        <v>0.17291666666666669</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2172,16 +2113,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2">
-        <v>0.18472222222222223</v>
+        <v>0.17222222222222225</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2193,16 +2134,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>9.0972222222222218E-2</v>
+        <v>0.14305555555555557</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2214,16 +2155,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>0.21180555555555555</v>
+        <v>0.18194444444444444</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2231,42 +2172,16 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.1173611111111111</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.16597222222222222</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>

</xml_diff>

<commit_message>
11080045 added review fl js ls
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="lauramvula3" localSheetId="0">Sheet1!$A$1:$E$11</definedName>
-    <definedName name="lauramvula3" localSheetId="2">Sheet3!$A$1:$E$11</definedName>
+    <definedName name="littlesimz2" localSheetId="0">Sheet1!$A$1:$E$20</definedName>
+    <definedName name="littlesimz2" localSheetId="2">Sheet3!$A$1:$E$20</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/lauramvula3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/littlesimz2.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/lauramvula3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/littlesimz2.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="37">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -75,43 +75,94 @@
     <t>Composer</t>
   </si>
   <si>
-    <t>Safe Passage</t>
-  </si>
-  <si>
-    <t>Laura Mvula, Dann Hume</t>
-  </si>
-  <si>
-    <t>Laura Mvula</t>
-  </si>
-  <si>
-    <t>Conditional</t>
-  </si>
-  <si>
-    <t>Church Girl</t>
-  </si>
-  <si>
-    <t>Remedy</t>
-  </si>
-  <si>
-    <t>Magical</t>
-  </si>
-  <si>
-    <t>Pink Noise</t>
-  </si>
-  <si>
-    <t>Golden Ashes</t>
-  </si>
-  <si>
-    <t>What Matters</t>
-  </si>
-  <si>
-    <t>Laura Mvul, Simon Neil</t>
-  </si>
-  <si>
-    <t>Got Me</t>
-  </si>
-  <si>
-    <t>Before the Dawn</t>
+    <t>Introvert</t>
+  </si>
+  <si>
+    <t>Simbiatu Ajikawo, Dean Josiah Cover</t>
+  </si>
+  <si>
+    <t>Little Simz</t>
+  </si>
+  <si>
+    <t>Woman</t>
+  </si>
+  <si>
+    <t>Simbiatu Ajikawo, Dean Josiah Cover, Cleopatra Nikolic</t>
+  </si>
+  <si>
+    <t>Little Simz feat. Cleo Sol</t>
+  </si>
+  <si>
+    <t>Two Worlds Apart</t>
+  </si>
+  <si>
+    <t>I Love You I Hate You</t>
+  </si>
+  <si>
+    <t>Little Q, Pt. 1 (Interlude)</t>
+  </si>
+  <si>
+    <t>Simbiatu Ajikawo, Dean Josiah Cover, Kadeem Clarke, Miles James</t>
+  </si>
+  <si>
+    <t>Little Q, Pt. 2</t>
+  </si>
+  <si>
+    <t>Gems (Interlude)</t>
+  </si>
+  <si>
+    <t>Simbiatu Ajikawo, Dean Josiah Cover, Kadeem Clarke</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Standing Ovation</t>
+  </si>
+  <si>
+    <t>I See You</t>
+  </si>
+  <si>
+    <t>Simbiatu Ajikawo, Dean Josiah Cover, Miles James, Nathan Allen</t>
+  </si>
+  <si>
+    <t>The Rapper That Came to Tea (Interlude)</t>
+  </si>
+  <si>
+    <t>Simbiatu Ajikawo, Dean Josiah Cover, Miles James, Kadeem Clarke</t>
+  </si>
+  <si>
+    <t>Rollin Stone</t>
+  </si>
+  <si>
+    <t>Simbiatu Ajikawo, Dean Josiah Cover, Miles James</t>
+  </si>
+  <si>
+    <t>Protect My Energy</t>
+  </si>
+  <si>
+    <t>Never Make Promises (Interlude)</t>
+  </si>
+  <si>
+    <t>Point and Kill</t>
+  </si>
+  <si>
+    <t>Simbiatu Ajikawo, Dean Josiah Cover, James Jacob</t>
+  </si>
+  <si>
+    <t>Fear No Man</t>
+  </si>
+  <si>
+    <t>Little Simz feat. Obongjayar</t>
+  </si>
+  <si>
+    <t>The Garden (Interlude)</t>
+  </si>
+  <si>
+    <t>How Did You Get Here</t>
+  </si>
+  <si>
+    <t>Miss Understood</t>
   </si>
 </sst>
 </file>
@@ -206,11 +257,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="lauramvula3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="littlesimz2" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="lauramvula3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="littlesimz2" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,10 +570,10 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="38.44140625" customWidth="1"/>
+    <col min="3" max="3" width="61.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
@@ -558,7 +609,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.13402777777777777</v>
+        <v>0.25208333333333333</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -573,13 +624,13 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2">
-        <v>0.1173611111111111</v>
+        <v>0.18680555555555556</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -591,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -600,7 +651,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15625</v>
+        <v>0.12361111111111112</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -612,7 +663,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -621,7 +672,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>0.16805555555555554</v>
+        <v>0.17708333333333334</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -633,16 +684,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>0.17500000000000002</v>
+        <v>4.7222222222222221E-2</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -654,16 +705,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>0.1451388888888889</v>
+        <v>0.15694444444444444</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -675,16 +726,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="2">
-        <v>0.17291666666666669</v>
+        <v>0.12291666666666667</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -696,16 +747,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.17222222222222225</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -717,7 +768,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -726,7 +777,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>0.14305555555555557</v>
+        <v>0.17222222222222225</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -738,16 +789,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>0.18194444444444444</v>
+        <v>0.16527777777777777</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -755,120 +806,247 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="E12" s="2"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.11458333333333333</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.15208333333333332</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.13055555555555556</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="E16" s="2"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.12847222222222224</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="5:10">
-      <c r="E17" s="2"/>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.16874999999999998</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="5:10">
-      <c r="E18" s="2"/>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.10972222222222222</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="5:10">
-      <c r="E19" s="2"/>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.20555555555555557</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="5:10">
-      <c r="E20" s="2"/>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.14375000000000002</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="5:10">
+    <row r="21" spans="1:10">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="5:10">
+    <row r="22" spans="1:10">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="5:10">
+    <row r="23" spans="1:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="5:10">
+    <row r="24" spans="1:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="5:10">
+    <row r="25" spans="1:10">
+      <c r="E25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="5:10">
+    <row r="26" spans="1:10">
+      <c r="E26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="5:10">
+    <row r="27" spans="1:10">
+      <c r="E27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="5:10">
+    <row r="28" spans="1:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="5:10">
+    <row r="29" spans="1:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="5:10">
+    <row r="30" spans="1:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="5:10">
+    <row r="31" spans="1:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="5:10">
+    <row r="32" spans="1:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">
@@ -882,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K27"/>
+  <dimension ref="A2:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="A3:K14"/>
+      <selection activeCell="K23" sqref="A3:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -905,15 +1083,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -933,21 +1111,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title          </v>
+        <v xml:space="preserve"> Title                                  </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers            </v>
+        <v xml:space="preserve"> Composers                                                     </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer             </v>
+        <v xml:space="preserve"> Performer                   </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -972,21 +1150,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">--------------- </v>
+        <v xml:space="preserve">--------------------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------- </v>
+        <v xml:space="preserve"> --------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------- </v>
+        <v xml:space="preserve"> ---------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1011,28 +1189,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Safe Passage   </v>
+        <v xml:space="preserve">Introvert                              </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover                            </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Laura Mvula           </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:13 </v>
+        <v xml:space="preserve">06:03 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1051,28 +1229,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Conditional    </v>
+        <v xml:space="preserve">Woman                                  </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover, Cleopatra Nikolic         </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Laura Mvula           </v>
+        <v xml:space="preserve">Little Simz feat. Cleo Sol  </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:49 </v>
+        <v xml:space="preserve">04:29 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1091,28 +1269,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Church Girl    </v>
+        <v xml:space="preserve">Two Worlds Apart                       </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover                            </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Laura Mvula           </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:45 </v>
+        <v xml:space="preserve">02:58 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1131,28 +1309,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Remedy         </v>
+        <v xml:space="preserve">I Love You I Hate You                  </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover                            </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Laura Mvula           </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:02 </v>
+        <v xml:space="preserve">04:15 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1171,28 +1349,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Magical        </v>
+        <v xml:space="preserve">Little Q, Pt. 1 (Interlude)            </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover, Kadeem Clarke, Miles James</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Laura Mvula           </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:12 </v>
+        <v xml:space="preserve">01:08 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1211,28 +1389,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Pink Noise     </v>
+        <v xml:space="preserve">Little Q, Pt. 2                        </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover, Kadeem Clarke, Miles James</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Laura Mvula           </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:29 </v>
+        <v xml:space="preserve">03:46 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1251,28 +1429,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Golden Ashes   </v>
+        <v xml:space="preserve">Gems (Interlude)                       </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover, Kadeem Clarke             </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Laura Mvula           </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:09 </v>
+        <v xml:space="preserve">02:57 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1291,28 +1469,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">What Matters   </v>
+        <v xml:space="preserve">Speed                                  </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover                            </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Laura Mvul, Simon Neil</v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:08 </v>
+        <v xml:space="preserve">02:40 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1331,28 +1509,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Got Me         </v>
+        <v xml:space="preserve">Standing Ovation                       </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover                            </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Laura Mvula           </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:26 </v>
+        <v xml:space="preserve">04:08 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1371,28 +1549,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Before the Dawn</v>
+        <v xml:space="preserve">I See You                              </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Laura Mvula, Dann Hume</v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover, Miles James, Nathan Allen </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Laura Mvula           </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:22 </v>
+        <v xml:space="preserve">03:58 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1404,35 +1582,35 @@
       </c>
       <c r="B15">
         <f>Sheet1!A12</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v>The Rapper That Came to Tea (Interlude)</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover, Miles James, Kadeem Clarke</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:45 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1444,35 +1622,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Rollin Stone                           </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover, Miles James               </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:39 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1484,35 +1662,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Protect My Energy                      </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover                            </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:08 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1524,35 +1702,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Never Make Promises (Interlude)        </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover                            </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">01:02 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1564,35 +1742,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Point and Kill                         </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover, James Jacob               </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:05 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1604,35 +1782,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Fear No Man                            </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover                            </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v>Little Simz feat. Obongjayar</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:03 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1644,35 +1822,35 @@
       </c>
       <c r="B21">
         <f>Sheet1!A18</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">The Garden (Interlude)                 </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover, Miles James, Kadeem Clarke</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:38 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
@@ -1684,35 +1862,35 @@
       </c>
       <c r="B22">
         <f>Sheet1!A19</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">How Did You Get Here                   </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover                            </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="3" t="str">
         <f>TEXT(Sheet1!E19,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:56 </v>
       </c>
       <c r="K22" s="4" t="s">
         <v>0</v>
@@ -1724,35 +1902,35 @@
       </c>
       <c r="B23">
         <f>Sheet1!A20</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Miss Understood                        </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve"> Simbiatu Ajikawo, Dean Josiah Cover                            </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">Little Simz                 </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J23" s="3" t="str">
         <f>TEXT(Sheet1!E20,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:27 </v>
       </c>
       <c r="K23" s="4" t="s">
         <v>0</v>
@@ -1771,21 +1949,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">                                       </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1811,21 +1989,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">                                       </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1851,21 +2029,21 @@
       </c>
       <c r="D26" t="str">
         <f>LEFTB(Sheet1!B23&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">                                       </v>
       </c>
       <c r="E26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="str">
         <f>" "&amp;LEFTB(Sheet1!C23&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H26" t="str">
         <f>LEFTB(Sheet1!D23&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I26" s="4" t="s">
         <v>0</v>
@@ -1891,21 +2069,21 @@
       </c>
       <c r="D27" t="str">
         <f>LEFTB(Sheet1!B24&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">                                       </v>
       </c>
       <c r="E27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="str">
         <f>" "&amp;LEFTB(Sheet1!C24&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H27" t="str">
         <f>LEFTB(Sheet1!D24&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I27" s="4" t="s">
         <v>0</v>
@@ -1915,6 +2093,246 @@
         <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K27" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <f>Sheet1!A25</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" t="str">
+        <f>LEFTB(Sheet1!B25&amp;REPT(" ",$D$2),$D$2)</f>
+        <v xml:space="preserve">                                       </v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" t="str">
+        <f>" "&amp;LEFTB(Sheet1!C25&amp;REPT(" ",$F$2),$F$2)</f>
+        <v xml:space="preserve">                                                                </v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" t="str">
+        <f>LEFTB(Sheet1!D25&amp;REPT(" ",$H$2),$H$2)</f>
+        <v xml:space="preserve">                            </v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3" t="str">
+        <f>TEXT(Sheet1!E25,"HH:MM")&amp;" "</f>
+        <v xml:space="preserve">00:00 </v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <f>Sheet1!A26</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" t="str">
+        <f>LEFTB(Sheet1!B26&amp;REPT(" ",$D$2),$D$2)</f>
+        <v xml:space="preserve">                                       </v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" t="str">
+        <f>" "&amp;LEFTB(Sheet1!C26&amp;REPT(" ",$F$2),$F$2)</f>
+        <v xml:space="preserve">                                                                </v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" t="str">
+        <f>LEFTB(Sheet1!D26&amp;REPT(" ",$H$2),$H$2)</f>
+        <v xml:space="preserve">                            </v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3" t="str">
+        <f>TEXT(Sheet1!E26,"HH:MM")&amp;" "</f>
+        <v xml:space="preserve">00:00 </v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <f>Sheet1!A27</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" t="str">
+        <f>LEFTB(Sheet1!B27&amp;REPT(" ",$D$2),$D$2)</f>
+        <v xml:space="preserve">                                       </v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" t="str">
+        <f>" "&amp;LEFTB(Sheet1!C27&amp;REPT(" ",$F$2),$F$2)</f>
+        <v xml:space="preserve">                                                                </v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" t="str">
+        <f>LEFTB(Sheet1!D27&amp;REPT(" ",$H$2),$H$2)</f>
+        <v xml:space="preserve">                            </v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3" t="str">
+        <f>TEXT(Sheet1!E27,"HH:MM")&amp;" "</f>
+        <v xml:space="preserve">00:00 </v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <f>Sheet1!A28</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" t="str">
+        <f>LEFTB(Sheet1!B28&amp;REPT(" ",$D$2),$D$2)</f>
+        <v xml:space="preserve">                                       </v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" t="str">
+        <f>" "&amp;LEFTB(Sheet1!C28&amp;REPT(" ",$F$2),$F$2)</f>
+        <v xml:space="preserve">                                                                </v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" t="str">
+        <f>LEFTB(Sheet1!D28&amp;REPT(" ",$H$2),$H$2)</f>
+        <v xml:space="preserve">                            </v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J31" s="3" t="str">
+        <f>TEXT(Sheet1!E28,"HH:MM")&amp;" "</f>
+        <v xml:space="preserve">00:00 </v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <f>Sheet1!A29</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" t="str">
+        <f>LEFTB(Sheet1!B29&amp;REPT(" ",$D$2),$D$2)</f>
+        <v xml:space="preserve">                                       </v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" t="str">
+        <f>" "&amp;LEFTB(Sheet1!C29&amp;REPT(" ",$F$2),$F$2)</f>
+        <v xml:space="preserve">                                                                </v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" t="str">
+        <f>LEFTB(Sheet1!D29&amp;REPT(" ",$H$2),$H$2)</f>
+        <v xml:space="preserve">                            </v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J32" s="3" t="str">
+        <f>TEXT(Sheet1!E29,"HH:MM")&amp;" "</f>
+        <v xml:space="preserve">00:00 </v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <f>Sheet1!A30</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" t="str">
+        <f>LEFTB(Sheet1!B30&amp;REPT(" ",$D$2),$D$2)</f>
+        <v xml:space="preserve">                                       </v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" t="str">
+        <f>" "&amp;LEFTB(Sheet1!C30&amp;REPT(" ",$F$2),$F$2)</f>
+        <v xml:space="preserve">                                                                </v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" t="str">
+        <f>LEFTB(Sheet1!D30&amp;REPT(" ",$H$2),$H$2)</f>
+        <v xml:space="preserve">                            </v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J33" s="3" t="str">
+        <f>TEXT(Sheet1!E30,"HH:MM")&amp;" "</f>
+        <v xml:space="preserve">00:00 </v>
+      </c>
+      <c r="K33" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1936,10 +2354,10 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="38.44140625" customWidth="1"/>
+    <col min="3" max="3" width="61.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
@@ -1975,7 +2393,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.13402777777777777</v>
+        <v>0.25208333333333333</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1990,13 +2408,13 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2">
-        <v>0.1173611111111111</v>
+        <v>0.18680555555555556</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2008,7 +2426,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -2017,7 +2435,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15625</v>
+        <v>0.12361111111111112</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2029,7 +2447,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -2038,7 +2456,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>0.16805555555555554</v>
+        <v>0.17708333333333334</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2050,16 +2468,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>0.17500000000000002</v>
+        <v>4.7222222222222221E-2</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2071,16 +2489,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>0.1451388888888889</v>
+        <v>0.15694444444444444</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2092,16 +2510,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="2">
-        <v>0.17291666666666669</v>
+        <v>0.12291666666666667</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2113,16 +2531,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.17222222222222225</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2134,7 +2552,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -2143,7 +2561,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>0.14305555555555557</v>
+        <v>0.17222222222222225</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2155,16 +2573,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>0.18194444444444444</v>
+        <v>0.16527777777777777</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2172,120 +2590,247 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="E12" s="2"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.11458333333333333</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.15208333333333332</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.13055555555555556</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="E16" s="2"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.12847222222222224</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="5:10">
-      <c r="E17" s="2"/>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.16874999999999998</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="5:10">
-      <c r="E18" s="2"/>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.10972222222222222</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="5:10">
-      <c r="E19" s="2"/>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.20555555555555557</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="5:10">
-      <c r="E20" s="2"/>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.14375000000000002</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="5:10">
+    <row r="21" spans="1:10">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="5:10">
+    <row r="22" spans="1:10">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="5:10">
+    <row r="23" spans="1:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="5:10">
+    <row r="24" spans="1:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="5:10">
+    <row r="25" spans="1:10">
+      <c r="E25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="5:10">
+    <row r="26" spans="1:10">
+      <c r="E26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="5:10">
+    <row r="27" spans="1:10">
+      <c r="E27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="5:10">
+    <row r="28" spans="1:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="5:10">
+    <row r="29" spans="1:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="5:10">
+    <row r="30" spans="1:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="5:10">
+    <row r="31" spans="1:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="5:10">
+    <row r="32" spans="1:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">

</xml_diff>

<commit_message>
12252225 added review lb vj rw
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="dawnrichard1" localSheetId="0">Sheet1!$A$1:$E$17</definedName>
-    <definedName name="dawnrichard1" localSheetId="2">Sheet3!$A$1:$E$17</definedName>
+    <definedName name="remiwolf1" localSheetId="0">Sheet1!$A$1:$E$14</definedName>
+    <definedName name="remiwolf1" localSheetId="2">Sheet3!$A$1:$E$14</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/dawnrichard1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/remiwolf1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/dawnrichard1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/remiwolf1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="31">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -75,70 +75,76 @@
     <t>Composer</t>
   </si>
   <si>
-    <t>King Creole (Intro)</t>
-  </si>
-  <si>
-    <t>Dawn Richard</t>
-  </si>
-  <si>
-    <t>Nostalgia</t>
-  </si>
-  <si>
-    <t>Boomerang</t>
-  </si>
-  <si>
-    <t>Dawn Richard feat. T.J., David Jy Lee</t>
-  </si>
-  <si>
-    <t>Bussifame</t>
-  </si>
-  <si>
-    <t>Pressure</t>
-  </si>
-  <si>
-    <t>Pilot (A Lude)</t>
-  </si>
-  <si>
-    <t>Jacuzzi</t>
-  </si>
-  <si>
-    <t>FiveOhFour (A Lude)</t>
-  </si>
-  <si>
-    <t>Voodoo (Intermission)</t>
-  </si>
-  <si>
-    <t>Mornin/Streetlights</t>
-  </si>
-  <si>
-    <t>Dawn Richard feat. Niko Galaura,T.J.</t>
-  </si>
-  <si>
-    <t>Le Petit Morte (A Lude)</t>
-  </si>
-  <si>
-    <t>Dawn Richard faet. Frank Richard</t>
-  </si>
-  <si>
-    <t>Radio Free</t>
-  </si>
-  <si>
-    <t>The Potter</t>
-  </si>
-  <si>
-    <t>Dawn Richard feat. Korina Marie, Omnel.FM</t>
-  </si>
-  <si>
-    <t>Perfect Storm</t>
-  </si>
-  <si>
-    <t>Dawn Richard feat. Korina Marie, Maem Aurum</t>
-  </si>
-  <si>
-    <t>Voodoo (Outermission)</t>
-  </si>
-  <si>
-    <t>Selfish (Outro)</t>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Liquor Store</t>
+  </si>
+  <si>
+    <t>Jared Solomon, Remi Wolf</t>
+  </si>
+  <si>
+    <t>Remi Wolf</t>
+  </si>
+  <si>
+    <t>Anthony Kiedis</t>
+  </si>
+  <si>
+    <t>wyd</t>
+  </si>
+  <si>
+    <t>Guerrilla</t>
+  </si>
+  <si>
+    <t>Quiet On Set</t>
+  </si>
+  <si>
+    <t>Jared Solomon, Remi Wolf, Elly Jay Rizk</t>
+  </si>
+  <si>
+    <t>Volkaino</t>
+  </si>
+  <si>
+    <t>Jared Solomon, Remi Wolf, Ari Starace</t>
+  </si>
+  <si>
+    <t>Front Tooth</t>
+  </si>
+  <si>
+    <t>Jared Solomon, Remi Wolf, Kenneth Charles Blume III</t>
+  </si>
+  <si>
+    <t>Grumpy Old Man</t>
+  </si>
+  <si>
+    <t>Jared Solomon, Remi Wolf, Ellas McDaniel</t>
+  </si>
+  <si>
+    <t>Buttermilk</t>
+  </si>
+  <si>
+    <t>Sally</t>
+  </si>
+  <si>
+    <t>Jared Solomon, Remi Wolf, Jullian McClanahan</t>
+  </si>
+  <si>
+    <t>Sexy Villain</t>
+  </si>
+  <si>
+    <t>Jared Solomon, Remi Wolf, Mark Landon, Mary Weltz, Olivia Waithe</t>
+  </si>
+  <si>
+    <t>Buzz Me In</t>
+  </si>
+  <si>
+    <t>Remi Wolf, Mark Landon, Mary Weltz, Olivia Waithe</t>
+  </si>
+  <si>
+    <t>Street You Live On</t>
+  </si>
+  <si>
+    <t>Remi Wolf, Ethan Gruska</t>
   </si>
 </sst>
 </file>
@@ -233,11 +239,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dawnrichard1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="remiwolf1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dawnrichard1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="remiwolf1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -540,16 +546,16 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E17"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="47.88671875" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="45.44140625" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="61.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
@@ -558,6 +564,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -576,16 +585,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>5.486111111111111E-2</v>
+        <v>0.11944444444444445</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -597,16 +606,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2">
-        <v>0.125</v>
+        <v>0.11875000000000001</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -618,16 +627,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2">
-        <v>0.1277777777777778</v>
+        <v>0.13819444444444443</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -639,16 +648,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2">
-        <v>0.18958333333333333</v>
+        <v>0.11388888888888889</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -660,16 +669,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2">
-        <v>0.17291666666666669</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -681,16 +690,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2">
-        <v>3.9583333333333331E-2</v>
+        <v>0.16319444444444445</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -702,16 +711,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13819444444444443</v>
+        <v>0.11458333333333333</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -723,16 +732,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
-        <v>5.0694444444444452E-2</v>
+        <v>0.14652777777777778</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -744,16 +753,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2">
-        <v>6.6666666666666666E-2</v>
+        <v>9.5138888888888884E-2</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -765,16 +774,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2">
-        <v>0.28125</v>
+        <v>0.11319444444444444</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -786,16 +795,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2">
-        <v>6.25E-2</v>
+        <v>0.13055555555555556</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -807,16 +816,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E13" s="5">
-        <v>8.3333333333333329E-2</v>
+        <v>0.11527777777777777</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
@@ -828,16 +837,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2">
-        <v>0.12013888888888889</v>
+        <v>0.14791666666666667</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -845,69 +854,27 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.23402777777777781</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="2">
-        <v>9.1666666666666674E-2</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.38125000000000003</v>
-      </c>
+    <row r="17" spans="5:10">
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="5:10">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -915,7 +882,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="5:10">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -923,64 +890,64 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="5:10">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="5:10">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="5:10">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="5:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="5:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="5:10">
       <c r="E25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="5:10">
       <c r="E26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="5:10">
       <c r="E27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="5:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="5:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="5:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="5:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="5:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">
@@ -997,7 +964,7 @@
   <dimension ref="A2:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="A3:K20"/>
+      <selection activeCell="K17" sqref="A3:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -1017,15 +984,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -1045,21 +1012,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                  </v>
+        <v xml:space="preserve"> Title             </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers  </v>
+        <v xml:space="preserve"> Composers                                                      </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                                  </v>
+        <v xml:space="preserve"> Performer</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1084,21 +1051,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">----------------------- </v>
+        <v xml:space="preserve">------------------ </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------ </v>
+        <v xml:space="preserve"> ---------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------- </v>
+        <v xml:space="preserve"> --------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1123,28 +1090,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">King Creole (Intro)    </v>
+        <v xml:space="preserve">Liquor Store      </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve"> Jared Solomon, Remi Wolf                                        </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard                               </v>
+        <v>Remi Wolf</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:19 </v>
+        <v xml:space="preserve">02:52 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1163,28 +1130,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Nostalgia              </v>
+        <v xml:space="preserve">Anthony Kiedis    </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve"> Jared Solomon, Remi Wolf                                        </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard                               </v>
+        <v>Remi Wolf</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:00 </v>
+        <v xml:space="preserve">02:51 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1203,28 +1170,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Boomerang              </v>
+        <v xml:space="preserve">wyd               </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve"> Jared Solomon, Remi Wolf                                        </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard feat. T.J., David Jy Lee      </v>
+        <v>Remi Wolf</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:04 </v>
+        <v xml:space="preserve">03:19 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1243,28 +1210,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Bussifame              </v>
+        <v xml:space="preserve">Guerrilla         </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve"> Jared Solomon, Remi Wolf                                        </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard                               </v>
+        <v>Remi Wolf</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:33 </v>
+        <v xml:space="preserve">02:44 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1283,28 +1250,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Pressure               </v>
+        <v xml:space="preserve">Quiet On Set      </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve"> Jared Solomon, Remi Wolf, Elly Jay Rizk                         </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard                               </v>
+        <v>Remi Wolf</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:09 </v>
+        <v xml:space="preserve">03:15 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1323,28 +1290,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Pilot (A Lude)         </v>
+        <v xml:space="preserve">Volkaino          </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve"> Jared Solomon, Remi Wolf, Ari Starace                           </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard                               </v>
+        <v>Remi Wolf</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:57 </v>
+        <v xml:space="preserve">03:55 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1363,28 +1330,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Jacuzzi                </v>
+        <v xml:space="preserve">Front Tooth       </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve"> Jared Solomon, Remi Wolf, Kenneth Charles Blume III             </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard                               </v>
+        <v>Remi Wolf</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:19 </v>
+        <v xml:space="preserve">02:45 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1403,28 +1370,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">FiveOhFour (A Lude)    </v>
+        <v xml:space="preserve">Grumpy Old Man    </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve"> Jared Solomon, Remi Wolf, Ellas McDaniel                        </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard                               </v>
+        <v>Remi Wolf</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:13 </v>
+        <v xml:space="preserve">03:31 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1443,28 +1410,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Voodoo (Intermission)  </v>
+        <v xml:space="preserve">Buttermilk        </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve"> Jared Solomon, Remi Wolf                                        </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard                               </v>
+        <v>Remi Wolf</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:36 </v>
+        <v xml:space="preserve">02:17 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1483,28 +1450,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Mornin/Streetlights    </v>
+        <v xml:space="preserve">Sally             </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve"> Jared Solomon, Remi Wolf, Jullian McClanahan                    </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard feat. Niko Galaura,T.J.       </v>
+        <v>Remi Wolf</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:45 </v>
+        <v xml:space="preserve">02:43 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1523,28 +1490,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Le Petit Morte (A Lude)</v>
+        <v xml:space="preserve">Sexy Villain      </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve"> Jared Solomon, Remi Wolf, Mark Landon, Mary Weltz, Olivia Waithe</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard faet. Frank Richard           </v>
+        <v>Remi Wolf</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:30 </v>
+        <v xml:space="preserve">03:08 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1563,28 +1530,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Radio Free             </v>
+        <v xml:space="preserve">Buzz Me In        </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve"> Remi Wolf, Mark Landon, Mary Weltz, Olivia Waithe               </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard                               </v>
+        <v>Remi Wolf</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:00 </v>
+        <v xml:space="preserve">02:46 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1603,28 +1570,28 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">The Potter             </v>
+        <v>Street You Live On</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve"> Remi Wolf, Ethan Gruska                                         </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard feat. Korina Marie, Omnel.FM  </v>
+        <v>Remi Wolf</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:53 </v>
+        <v xml:space="preserve">03:33 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1636,35 +1603,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Perfect Storm          </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Dawn Richard feat. Korina Marie, Maem Aurum</v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:37 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1676,35 +1643,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Voodoo (Outermission)  </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard                               </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:12 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1716,35 +1683,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Selfish (Outro)        </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dawn Richard</v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dawn Richard                               </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">09:09 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1763,21 +1730,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1803,21 +1770,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1843,21 +1810,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1883,21 +1850,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1923,21 +1890,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1963,21 +1930,21 @@
       </c>
       <c r="D26" t="str">
         <f>LEFTB(Sheet1!B23&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="str">
         <f>" "&amp;LEFTB(Sheet1!C23&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H26" t="str">
         <f>LEFTB(Sheet1!D23&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I26" s="4" t="s">
         <v>0</v>
@@ -2003,21 +1970,21 @@
       </c>
       <c r="D27" t="str">
         <f>LEFTB(Sheet1!B24&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="str">
         <f>" "&amp;LEFTB(Sheet1!C24&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H27" t="str">
         <f>LEFTB(Sheet1!D24&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I27" s="4" t="s">
         <v>0</v>
@@ -2043,21 +2010,21 @@
       </c>
       <c r="D28" t="str">
         <f>LEFTB(Sheet1!B25&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F28" t="str">
         <f>" "&amp;LEFTB(Sheet1!C25&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H28" t="str">
         <f>LEFTB(Sheet1!D25&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I28" s="4" t="s">
         <v>0</v>
@@ -2083,21 +2050,21 @@
       </c>
       <c r="D29" t="str">
         <f>LEFTB(Sheet1!B26&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E29" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F29" t="str">
         <f>" "&amp;LEFTB(Sheet1!C26&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G29" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H29" t="str">
         <f>LEFTB(Sheet1!D26&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I29" s="4" t="s">
         <v>0</v>
@@ -2123,21 +2090,21 @@
       </c>
       <c r="D30" t="str">
         <f>LEFTB(Sheet1!B27&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F30" t="str">
         <f>" "&amp;LEFTB(Sheet1!C27&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H30" t="str">
         <f>LEFTB(Sheet1!D27&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I30" s="4" t="s">
         <v>0</v>
@@ -2163,21 +2130,21 @@
       </c>
       <c r="D31" t="str">
         <f>LEFTB(Sheet1!B28&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F31" t="str">
         <f>" "&amp;LEFTB(Sheet1!C28&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H31" t="str">
         <f>LEFTB(Sheet1!D28&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I31" s="4" t="s">
         <v>0</v>
@@ -2203,21 +2170,21 @@
       </c>
       <c r="D32" t="str">
         <f>LEFTB(Sheet1!B29&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F32" t="str">
         <f>" "&amp;LEFTB(Sheet1!C29&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H32" t="str">
         <f>LEFTB(Sheet1!D29&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I32" s="4" t="s">
         <v>0</v>
@@ -2243,21 +2210,21 @@
       </c>
       <c r="D33" t="str">
         <f>LEFTB(Sheet1!B30&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F33" t="str">
         <f>" "&amp;LEFTB(Sheet1!C30&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                 </v>
       </c>
       <c r="G33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H33" t="str">
         <f>LEFTB(Sheet1!D30&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="I33" s="4" t="s">
         <v>0</v>
@@ -2282,15 +2249,15 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E17"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="43.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="61.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
@@ -2300,6 +2267,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -2318,16 +2288,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>5.486111111111111E-2</v>
+        <v>0.11944444444444445</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2339,16 +2309,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2">
-        <v>0.125</v>
+        <v>0.11875000000000001</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2360,16 +2330,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2">
-        <v>0.1277777777777778</v>
+        <v>0.13819444444444443</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2381,16 +2351,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2">
-        <v>0.18958333333333333</v>
+        <v>0.11388888888888889</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2402,16 +2372,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2">
-        <v>0.17291666666666669</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2423,16 +2393,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2">
-        <v>3.9583333333333331E-2</v>
+        <v>0.16319444444444445</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2444,16 +2414,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13819444444444443</v>
+        <v>0.11458333333333333</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2465,16 +2435,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
-        <v>5.0694444444444452E-2</v>
+        <v>0.14652777777777778</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2486,16 +2456,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2">
-        <v>6.6666666666666666E-2</v>
+        <v>9.5138888888888884E-2</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2507,16 +2477,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2">
-        <v>0.28125</v>
+        <v>0.11319444444444444</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2528,16 +2498,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2">
-        <v>6.25E-2</v>
+        <v>0.13055555555555556</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2549,16 +2519,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E13" s="5">
-        <v>8.3333333333333329E-2</v>
+        <v>0.11527777777777777</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
@@ -2570,16 +2540,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2">
-        <v>0.12013888888888889</v>
+        <v>0.14791666666666667</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2587,69 +2557,27 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.23402777777777781</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="2">
-        <v>9.1666666666666674E-2</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.38125000000000003</v>
-      </c>
+    <row r="17" spans="5:10">
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="5:10">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -2657,7 +2585,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="5:10">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -2665,64 +2593,64 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="5:10">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="5:10">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="5:10">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="5:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="5:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="5:10">
       <c r="E25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="5:10">
       <c r="E26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="5:10">
       <c r="E27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="5:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="5:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="5:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="5:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="5:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">

</xml_diff>

<commit_message>
12312030 added review ln best50
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="remiwolf1" localSheetId="0">Sheet1!$A$1:$E$14</definedName>
-    <definedName name="remiwolf1" localSheetId="2">Sheet3!$A$1:$E$14</definedName>
+    <definedName name="lilnasx1" localSheetId="0">Sheet1!$A$1:$E$16</definedName>
+    <definedName name="lilnasx1" localSheetId="2">Sheet3!$A$1:$E$16</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/remiwolf1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/lilnasx1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/remiwolf1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/lilnasx1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="42">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -75,76 +75,109 @@
     <t>Composer</t>
   </si>
   <si>
-    <t>No.</t>
-  </si>
-  <si>
-    <t>Liquor Store</t>
-  </si>
-  <si>
-    <t>Jared Solomon, Remi Wolf</t>
-  </si>
-  <si>
-    <t>Remi Wolf</t>
-  </si>
-  <si>
-    <t>Anthony Kiedis</t>
-  </si>
-  <si>
-    <t>wyd</t>
-  </si>
-  <si>
-    <t>Guerrilla</t>
-  </si>
-  <si>
-    <t>Quiet On Set</t>
-  </si>
-  <si>
-    <t>Jared Solomon, Remi Wolf, Elly Jay Rizk</t>
-  </si>
-  <si>
-    <t>Volkaino</t>
-  </si>
-  <si>
-    <t>Jared Solomon, Remi Wolf, Ari Starace</t>
-  </si>
-  <si>
-    <t>Front Tooth</t>
-  </si>
-  <si>
-    <t>Jared Solomon, Remi Wolf, Kenneth Charles Blume III</t>
-  </si>
-  <si>
-    <t>Grumpy Old Man</t>
-  </si>
-  <si>
-    <t>Jared Solomon, Remi Wolf, Ellas McDaniel</t>
-  </si>
-  <si>
-    <t>Buttermilk</t>
-  </si>
-  <si>
-    <t>Sally</t>
-  </si>
-  <si>
-    <t>Jared Solomon, Remi Wolf, Jullian McClanahan</t>
-  </si>
-  <si>
-    <t>Sexy Villain</t>
-  </si>
-  <si>
-    <t>Jared Solomon, Remi Wolf, Mark Landon, Mary Weltz, Olivia Waithe</t>
-  </si>
-  <si>
-    <t>Buzz Me In</t>
-  </si>
-  <si>
-    <t>Remi Wolf, Mark Landon, Mary Weltz, Olivia Waithe</t>
-  </si>
-  <si>
-    <t>Street You Live On</t>
-  </si>
-  <si>
-    <t>Remi Wolf, Ethan Gruska</t>
+    <t>Montero (Call Me By Your Name)</t>
+  </si>
+  <si>
+    <t>Denzel Baptiste, David Biral, Omer Fedi, Roy Lenzo, Montero Hill</t>
+  </si>
+  <si>
+    <t>Lil Nas X</t>
+  </si>
+  <si>
+    <t>Dead Right Now</t>
+  </si>
+  <si>
+    <t>Denzel Baptiste, David Biral, Jasper Harris, Thomas James Levesque, Montero Hill</t>
+  </si>
+  <si>
+    <t>Industry Baby</t>
+  </si>
+  <si>
+    <t>Denzel Baptiste, David Biral, Jack Harlow, Nick Lee, Montero Hill, Kanye West</t>
+  </si>
+  <si>
+    <t>Lil Nas X &amp; Jack Harlow</t>
+  </si>
+  <si>
+    <t>Thats What I Want</t>
+  </si>
+  <si>
+    <t>Omer Fedi, Keegan Bach, Montero Hill, Blake Slatkin, Ryan Tedder</t>
+  </si>
+  <si>
+    <t>The Art of Realization</t>
+  </si>
+  <si>
+    <t>Denzel Baptiste, David Biral, Roy Lenzo, Montero Hill</t>
+  </si>
+  <si>
+    <t>Scoop</t>
+  </si>
+  <si>
+    <t>Amala Zandile Dlamini, Denzel Baptiste, David Biral, Roy Lenzo, Montero Hill</t>
+  </si>
+  <si>
+    <t>Lil Nas X feat. Doja Cat</t>
+  </si>
+  <si>
+    <t>One of Me</t>
+  </si>
+  <si>
+    <t>John Cunningham, Isley Juber, Montero Hill, Jasper Sheff</t>
+  </si>
+  <si>
+    <t>Lil Nas X feat. Elton John</t>
+  </si>
+  <si>
+    <t>Lost in the Citadel</t>
+  </si>
+  <si>
+    <t>John Cunningham, Montero Hill</t>
+  </si>
+  <si>
+    <t>Dolla Sign Slime</t>
+  </si>
+  <si>
+    <t>Denzel Baptiste, David Biral, Nick Lee, Megan Pete, Montero Hill</t>
+  </si>
+  <si>
+    <t>Lil Nas X feat. Megan thee Stallion</t>
+  </si>
+  <si>
+    <t>Tales of Dominica</t>
+  </si>
+  <si>
+    <t>Sun Goes Down</t>
+  </si>
+  <si>
+    <t>Denzel Baptiste, David Biral, Omer Fedi, Keegan Bach, Roy Lenzo, Andrew Luce, Montero Hill, Michael Olmo, Blake Slatkin</t>
+  </si>
+  <si>
+    <t>Void</t>
+  </si>
+  <si>
+    <t>John Cunningham, Carter Lang, Montero Hill</t>
+  </si>
+  <si>
+    <t>Don't Want It</t>
+  </si>
+  <si>
+    <t>Denzel Baptiste, David Biral, Nicholas Mira, Montero Hill, Dorien Theus</t>
+  </si>
+  <si>
+    <t>Life After Salem</t>
+  </si>
+  <si>
+    <t>John Cunningham, Carter Lang, Montero Hill, Jasper Sheff</t>
+  </si>
+  <si>
+    <t>Am I Dreaming</t>
+  </si>
+  <si>
+    <t>Denzel Baptiste, David Biral, Miley Cyrus, Omer Fedi, Vincent Goodyer, Montero Hill, William K Ward</t>
+  </si>
+  <si>
+    <t>Lil Nas X feat. Miley Cyrus</t>
   </si>
 </sst>
 </file>
@@ -239,11 +272,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="remiwolf1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="lilnasx1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="remiwolf1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="lilnasx1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -551,10 +584,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="61.77734375" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
@@ -564,9 +597,6 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -585,16 +615,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="2">
-        <v>0.11944444444444445</v>
+        <v>9.5833333333333326E-2</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -606,16 +636,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.11875000000000001</v>
+        <v>0.15347222222222223</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -630,13 +660,13 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>0.13819444444444443</v>
+        <v>0.14722222222222223</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -648,16 +678,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
       <c r="E5" s="2">
-        <v>0.11388888888888889</v>
+        <v>9.930555555555555E-2</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -669,16 +699,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13541666666666666</v>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -690,16 +720,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2">
-        <v>0.16319444444444445</v>
+        <v>0.12083333333333333</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -711,16 +741,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E8" s="2">
-        <v>0.11458333333333333</v>
+        <v>0.1125</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -732,16 +762,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.14652777777777778</v>
+        <v>0.11805555555555557</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -753,16 +783,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2">
-        <v>9.5138888888888884E-2</v>
+        <v>0.10069444444444443</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -774,16 +804,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>0.11319444444444444</v>
+        <v>0.1013888888888889</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -795,16 +825,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2">
-        <v>0.13055555555555556</v>
+        <v>0.11666666666666665</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -816,16 +846,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="5">
-        <v>0.11527777777777777</v>
+        <v>0.17222222222222225</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
@@ -837,16 +867,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" s="2">
-        <v>0.14791666666666667</v>
+        <v>9.1666666666666674E-2</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -854,14 +884,42 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.14652777777777778</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="E16" s="2"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.12708333333333333</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -964,7 +1022,7 @@
   <dimension ref="A2:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="A3:K17"/>
+      <selection activeCell="K19" sqref="A3:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -984,15 +1042,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -1012,21 +1070,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title             </v>
+        <v xml:space="preserve"> Title                         </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                      </v>
+        <v xml:space="preserve"> Composers                                                                                                             </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer</v>
+        <v xml:space="preserve"> Performer                          </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1051,21 +1109,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------ </v>
+        <v xml:space="preserve">------------------------------ </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> --------- </v>
+        <v xml:space="preserve"> ----------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1090,28 +1148,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Liquor Store      </v>
+        <v>Montero (Call Me By Your Name)</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jared Solomon, Remi Wolf                                        </v>
+        <v xml:space="preserve"> Denzel Baptiste, David Biral, Omer Fedi, Roy Lenzo, Montero Hill                                                       </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Remi Wolf</v>
+        <v xml:space="preserve">Lil Nas X                          </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:52 </v>
+        <v xml:space="preserve">02:18 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1130,28 +1188,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Anthony Kiedis    </v>
+        <v xml:space="preserve">Dead Right Now                </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jared Solomon, Remi Wolf                                        </v>
+        <v xml:space="preserve"> Denzel Baptiste, David Biral, Jasper Harris, Thomas James Levesque, Montero Hill                                       </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Remi Wolf</v>
+        <v xml:space="preserve">Lil Nas X                          </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:51 </v>
+        <v xml:space="preserve">03:41 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1170,28 +1228,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">wyd               </v>
+        <v xml:space="preserve">Industry Baby                 </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jared Solomon, Remi Wolf                                        </v>
+        <v xml:space="preserve"> Denzel Baptiste, David Biral, Jack Harlow, Nick Lee, Montero Hill, Kanye West                                          </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Remi Wolf</v>
+        <v xml:space="preserve">Lil Nas X &amp; Jack Harlow            </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:19 </v>
+        <v xml:space="preserve">03:32 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1210,28 +1268,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Guerrilla         </v>
+        <v xml:space="preserve">Thats What I Want             </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jared Solomon, Remi Wolf                                        </v>
+        <v xml:space="preserve"> Omer Fedi, Keegan Bach, Montero Hill, Blake Slatkin, Ryan Tedder                                                       </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Remi Wolf</v>
+        <v xml:space="preserve">Lil Nas X                          </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:44 </v>
+        <v xml:space="preserve">02:23 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1250,28 +1308,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Quiet On Set      </v>
+        <v xml:space="preserve">The Art of Realization        </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jared Solomon, Remi Wolf, Elly Jay Rizk                         </v>
+        <v xml:space="preserve"> Denzel Baptiste, David Biral, Roy Lenzo, Montero Hill                                                                  </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Remi Wolf</v>
+        <v xml:space="preserve">Lil Nas X                          </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:15 </v>
+        <v xml:space="preserve">00:24 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1290,28 +1348,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Volkaino          </v>
+        <v xml:space="preserve">Scoop                         </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jared Solomon, Remi Wolf, Ari Starace                           </v>
+        <v xml:space="preserve"> Amala Zandile Dlamini, Denzel Baptiste, David Biral, Roy Lenzo, Montero Hill                                           </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Remi Wolf</v>
+        <v xml:space="preserve">Lil Nas X feat. Doja Cat           </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:55 </v>
+        <v xml:space="preserve">02:54 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1330,28 +1388,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Front Tooth       </v>
+        <v xml:space="preserve">One of Me                     </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jared Solomon, Remi Wolf, Kenneth Charles Blume III             </v>
+        <v xml:space="preserve"> John Cunningham, Isley Juber, Montero Hill, Jasper Sheff                                                               </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Remi Wolf</v>
+        <v xml:space="preserve">Lil Nas X feat. Elton John         </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:45 </v>
+        <v xml:space="preserve">02:42 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1370,28 +1428,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Grumpy Old Man    </v>
+        <v xml:space="preserve">Lost in the Citadel           </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jared Solomon, Remi Wolf, Ellas McDaniel                        </v>
+        <v xml:space="preserve"> John Cunningham, Montero Hill                                                                                          </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Remi Wolf</v>
+        <v xml:space="preserve">Lil Nas X                          </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:31 </v>
+        <v xml:space="preserve">02:50 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1410,28 +1468,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Buttermilk        </v>
+        <v xml:space="preserve">Dolla Sign Slime              </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jared Solomon, Remi Wolf                                        </v>
+        <v xml:space="preserve"> Denzel Baptiste, David Biral, Nick Lee, Megan Pete, Montero Hill                                                       </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Remi Wolf</v>
+        <v>Lil Nas X feat. Megan thee Stallion</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:17 </v>
+        <v xml:space="preserve">02:25 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1450,28 +1508,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sally             </v>
+        <v xml:space="preserve">Tales of Dominica             </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jared Solomon, Remi Wolf, Jullian McClanahan                    </v>
+        <v xml:space="preserve"> Denzel Baptiste, David Biral, Omer Fedi, Roy Lenzo, Montero Hill                                                       </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Remi Wolf</v>
+        <v xml:space="preserve">Lil Nas X                          </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:43 </v>
+        <v xml:space="preserve">02:26 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1490,28 +1548,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sexy Villain      </v>
+        <v xml:space="preserve">Sun Goes Down                 </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jared Solomon, Remi Wolf, Mark Landon, Mary Weltz, Olivia Waithe</v>
+        <v xml:space="preserve"> Denzel Baptiste, David Biral, Omer Fedi, Keegan Bach, Roy Lenzo, Andrew Luce, Montero Hill, Michael Olmo, Blake Slatkin</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Remi Wolf</v>
+        <v xml:space="preserve">Lil Nas X                          </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:08 </v>
+        <v xml:space="preserve">02:48 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1530,28 +1588,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Buzz Me In        </v>
+        <v xml:space="preserve">Void                          </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Remi Wolf, Mark Landon, Mary Weltz, Olivia Waithe               </v>
+        <v xml:space="preserve"> John Cunningham, Carter Lang, Montero Hill                                                                             </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Remi Wolf</v>
+        <v xml:space="preserve">Lil Nas X                          </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:46 </v>
+        <v xml:space="preserve">04:08 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1570,28 +1628,28 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Street You Live On</v>
+        <v xml:space="preserve">Don't Want It                 </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Remi Wolf, Ethan Gruska                                         </v>
+        <v xml:space="preserve"> Denzel Baptiste, David Biral, Nicholas Mira, Montero Hill, Dorien Theus                                                </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Remi Wolf</v>
+        <v xml:space="preserve">Lil Nas X                          </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:33 </v>
+        <v xml:space="preserve">02:12 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1603,35 +1661,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Life After Salem              </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve"> John Cunningham, Carter Lang, Montero Hill, Jasper Sheff                                                               </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">Lil Nas X                          </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:31 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1643,35 +1701,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Am I Dreaming                 </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve"> Denzel Baptiste, David Biral, Miley Cyrus, Omer Fedi, Vincent Goodyer, Montero Hill, William K Ward                    </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">Lil Nas X feat. Miley Cyrus        </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:03 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1690,21 +1748,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1730,21 +1788,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1770,21 +1828,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1810,21 +1868,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1850,21 +1908,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1890,21 +1948,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1930,21 +1988,21 @@
       </c>
       <c r="D26" t="str">
         <f>LEFTB(Sheet1!B23&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="str">
         <f>" "&amp;LEFTB(Sheet1!C23&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H26" t="str">
         <f>LEFTB(Sheet1!D23&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I26" s="4" t="s">
         <v>0</v>
@@ -1970,21 +2028,21 @@
       </c>
       <c r="D27" t="str">
         <f>LEFTB(Sheet1!B24&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="str">
         <f>" "&amp;LEFTB(Sheet1!C24&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H27" t="str">
         <f>LEFTB(Sheet1!D24&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I27" s="4" t="s">
         <v>0</v>
@@ -2010,21 +2068,21 @@
       </c>
       <c r="D28" t="str">
         <f>LEFTB(Sheet1!B25&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F28" t="str">
         <f>" "&amp;LEFTB(Sheet1!C25&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H28" t="str">
         <f>LEFTB(Sheet1!D25&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I28" s="4" t="s">
         <v>0</v>
@@ -2050,21 +2108,21 @@
       </c>
       <c r="D29" t="str">
         <f>LEFTB(Sheet1!B26&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E29" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F29" t="str">
         <f>" "&amp;LEFTB(Sheet1!C26&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G29" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H29" t="str">
         <f>LEFTB(Sheet1!D26&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I29" s="4" t="s">
         <v>0</v>
@@ -2090,21 +2148,21 @@
       </c>
       <c r="D30" t="str">
         <f>LEFTB(Sheet1!B27&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F30" t="str">
         <f>" "&amp;LEFTB(Sheet1!C27&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H30" t="str">
         <f>LEFTB(Sheet1!D27&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I30" s="4" t="s">
         <v>0</v>
@@ -2130,21 +2188,21 @@
       </c>
       <c r="D31" t="str">
         <f>LEFTB(Sheet1!B28&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F31" t="str">
         <f>" "&amp;LEFTB(Sheet1!C28&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H31" t="str">
         <f>LEFTB(Sheet1!D28&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I31" s="4" t="s">
         <v>0</v>
@@ -2170,21 +2228,21 @@
       </c>
       <c r="D32" t="str">
         <f>LEFTB(Sheet1!B29&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F32" t="str">
         <f>" "&amp;LEFTB(Sheet1!C29&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H32" t="str">
         <f>LEFTB(Sheet1!D29&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I32" s="4" t="s">
         <v>0</v>
@@ -2210,21 +2268,21 @@
       </c>
       <c r="D33" t="str">
         <f>LEFTB(Sheet1!B30&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F33" t="str">
         <f>" "&amp;LEFTB(Sheet1!C30&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                 </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H33" t="str">
         <f>LEFTB(Sheet1!D30&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I33" s="4" t="s">
         <v>0</v>
@@ -2254,10 +2312,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="61.77734375" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
@@ -2267,9 +2325,6 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -2288,16 +2343,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="2">
-        <v>0.11944444444444445</v>
+        <v>9.5833333333333326E-2</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2309,16 +2364,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.11875000000000001</v>
+        <v>0.15347222222222223</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2333,13 +2388,13 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>0.13819444444444443</v>
+        <v>0.14722222222222223</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2351,16 +2406,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
       <c r="E5" s="2">
-        <v>0.11388888888888889</v>
+        <v>9.930555555555555E-2</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2372,16 +2427,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13541666666666666</v>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2393,16 +2448,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2">
-        <v>0.16319444444444445</v>
+        <v>0.12083333333333333</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2414,16 +2469,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E8" s="2">
-        <v>0.11458333333333333</v>
+        <v>0.1125</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2435,16 +2490,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.14652777777777778</v>
+        <v>0.11805555555555557</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2456,16 +2511,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2">
-        <v>9.5138888888888884E-2</v>
+        <v>0.10069444444444443</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2477,16 +2532,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>0.11319444444444444</v>
+        <v>0.1013888888888889</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2498,16 +2553,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2">
-        <v>0.13055555555555556</v>
+        <v>0.11666666666666665</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2519,16 +2574,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="5">
-        <v>0.11527777777777777</v>
+        <v>0.17222222222222225</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
@@ -2540,16 +2595,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" s="2">
-        <v>0.14791666666666667</v>
+        <v>9.1666666666666674E-2</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2557,14 +2612,42 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.14652777777777778</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="E16" s="2"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.12708333333333333</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>

</xml_diff>

<commit_message>
011620 05 added reviewad dr
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,10 +17,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="lilnasx1" localSheetId="0">Sheet1!$A$1:$E$16</definedName>
-    <definedName name="lilnasx1" localSheetId="2">Sheet3!$A$1:$E$16</definedName>
+    <definedName name="drake8" localSheetId="0">Sheet1!$A$1:$E$22</definedName>
+    <definedName name="drake8" localSheetId="2">Sheet3!$A$1:$E$22</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,14 +33,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/lilnasx1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/drake8.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/lilnasx1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/drake8.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="62">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -75,109 +76,169 @@
     <t>Composer</t>
   </si>
   <si>
-    <t>Montero (Call Me By Your Name)</t>
-  </si>
-  <si>
-    <t>Denzel Baptiste, David Biral, Omer Fedi, Roy Lenzo, Montero Hill</t>
-  </si>
-  <si>
-    <t>Lil Nas X</t>
-  </si>
-  <si>
-    <t>Dead Right Now</t>
-  </si>
-  <si>
-    <t>Denzel Baptiste, David Biral, Jasper Harris, Thomas James Levesque, Montero Hill</t>
-  </si>
-  <si>
-    <t>Industry Baby</t>
-  </si>
-  <si>
-    <t>Denzel Baptiste, David Biral, Jack Harlow, Nick Lee, Montero Hill, Kanye West</t>
-  </si>
-  <si>
-    <t>Lil Nas X &amp; Jack Harlow</t>
-  </si>
-  <si>
-    <t>Thats What I Want</t>
-  </si>
-  <si>
-    <t>Omer Fedi, Keegan Bach, Montero Hill, Blake Slatkin, Ryan Tedder</t>
-  </si>
-  <si>
-    <t>The Art of Realization</t>
-  </si>
-  <si>
-    <t>Denzel Baptiste, David Biral, Roy Lenzo, Montero Hill</t>
-  </si>
-  <si>
-    <t>Scoop</t>
-  </si>
-  <si>
-    <t>Amala Zandile Dlamini, Denzel Baptiste, David Biral, Roy Lenzo, Montero Hill</t>
-  </si>
-  <si>
-    <t>Lil Nas X feat. Doja Cat</t>
-  </si>
-  <si>
-    <t>One of Me</t>
-  </si>
-  <si>
-    <t>John Cunningham, Isley Juber, Montero Hill, Jasper Sheff</t>
-  </si>
-  <si>
-    <t>Lil Nas X feat. Elton John</t>
-  </si>
-  <si>
-    <t>Lost in the Citadel</t>
-  </si>
-  <si>
-    <t>John Cunningham, Montero Hill</t>
-  </si>
-  <si>
-    <t>Dolla Sign Slime</t>
-  </si>
-  <si>
-    <t>Denzel Baptiste, David Biral, Nick Lee, Megan Pete, Montero Hill</t>
-  </si>
-  <si>
-    <t>Lil Nas X feat. Megan thee Stallion</t>
-  </si>
-  <si>
-    <t>Tales of Dominica</t>
-  </si>
-  <si>
-    <t>Sun Goes Down</t>
-  </si>
-  <si>
-    <t>Denzel Baptiste, David Biral, Omer Fedi, Keegan Bach, Roy Lenzo, Andrew Luce, Montero Hill, Michael Olmo, Blake Slatkin</t>
-  </si>
-  <si>
-    <t>Void</t>
-  </si>
-  <si>
-    <t>John Cunningham, Carter Lang, Montero Hill</t>
-  </si>
-  <si>
-    <t>Don't Want It</t>
-  </si>
-  <si>
-    <t>Denzel Baptiste, David Biral, Nicholas Mira, Montero Hill, Dorien Theus</t>
-  </si>
-  <si>
-    <t>Life After Salem</t>
-  </si>
-  <si>
-    <t>John Cunningham, Carter Lang, Montero Hill, Jasper Sheff</t>
-  </si>
-  <si>
-    <t>Am I Dreaming</t>
-  </si>
-  <si>
-    <t>Denzel Baptiste, David Biral, Miley Cyrus, Omer Fedi, Vincent Goodyer, Montero Hill, William K Ward</t>
-  </si>
-  <si>
-    <t>Lil Nas X feat. Miley Cyrus</t>
+    <t>Champagne Poetry</t>
+  </si>
+  <si>
+    <t>Maneesh Bidaye / Micah Davis / Aubrey Graham / Gabriel Hardeman / Jean-Andre Lawrence / John Lennon / Paul McCartney / Noah Shebib</t>
+  </si>
+  <si>
+    <t>Drake</t>
+  </si>
+  <si>
+    <t>Papi’s Home</t>
+  </si>
+  <si>
+    <t>Mark Borino / Anthony "Shep" Crawford / Aubrey Graham / Raynford Humphrey / Montell Jordan / Michael Gordon Jr. / Oriyomi Ojelade / Jonathan D. Priester / Jarrel Young</t>
+  </si>
+  <si>
+    <t>Girls Want Girls</t>
+  </si>
+  <si>
+    <t>Aubrey Graham / Dominique Jones / Mathias Liyew / Ozan Yildirim</t>
+  </si>
+  <si>
+    <t>Drake feat: Lil Baby</t>
+  </si>
+  <si>
+    <t>In the Bible</t>
+  </si>
+  <si>
+    <t>Durk Banks / Eli Brown / Eliel Brown / Giveon Evans / Simon Gebrelul / Giveon / Aubrey Graham / Leon Thomas III / Austin Schindler / Noah Shebib</t>
+  </si>
+  <si>
+    <t>Drake feat: Lil Durk / Giveon</t>
+  </si>
+  <si>
+    <t>Love All</t>
+  </si>
+  <si>
+    <t>Shawn Carter / Dylan Cleary-Krell / Luke Combs / Sean Combs / Aubrey Graham / Leon Thomas III / Majid Jordan / Steven Jordan / Khristopher Riddick-Tynes / Christopher Wallace / Ozan Yildirim</t>
+  </si>
+  <si>
+    <t>Drake feat: Jay-Z</t>
+  </si>
+  <si>
+    <t>Fair Trade</t>
+  </si>
+  <si>
+    <t>Reibaldi Sephane Antoine / Brandon Banks / Kenneth Edmonds / Aubrey Graham / Teo Halm / Dernst Emile II / Michael Gordon Jr. / Kyla Moscovich / Ebony Oshunrinde / Marcus Reddick / Jahaan Sweet / Varren Wade / Jacques Webster / Charlotte Day Wilson / Ozan Yildirim</t>
+  </si>
+  <si>
+    <t>Drake feat: Travis Scott</t>
+  </si>
+  <si>
+    <t>Way 2 Sexy</t>
+  </si>
+  <si>
+    <t>Fred Fairbrass / Richard Fairbrass / Aubrey Graham / Rob Manzoli / Lesidney Ragland / Brandon Simmons / Bryan Simmons / Nayvadius Wilburn / Jeffery Williams</t>
+  </si>
+  <si>
+    <t>Drake feat: Future / Young Thug</t>
+  </si>
+  <si>
+    <t>TSU</t>
+  </si>
+  <si>
+    <t>Harley Arsenault / Noel Cadastre / Christopher Cross / Aubrey Graham / Nate Hills / Nathaniel Hills / R. Kelly / Robert Kelly / Timothy Mosley / Justin Timberlake</t>
+  </si>
+  <si>
+    <t>N 2 Deep</t>
+  </si>
+  <si>
+    <t>Harley Arsenault / Kaushik Barua / Chad Butler / Noel Cadastre / Shawn Carter / B. J. Freeman / Bernard Freeman / Aubrey Graham / Jay Jenkins / Leroy Williams, Jr. / Alex Lustig / Joseph McVey / Noah Shebib / Nayvadius Wilburn / Leroy Williams</t>
+  </si>
+  <si>
+    <t>Drake feat: Future</t>
+  </si>
+  <si>
+    <t>Pipe Down</t>
+  </si>
+  <si>
+    <t>Lazaro Camejo / Simon Gebrelul / Aubrey Graham / Abdelhady Moamer Hafez / Leon Thomas III / Robert E. Fairfax III / Derek Kastal / Anthoine Walters / Walters</t>
+  </si>
+  <si>
+    <t>Yebba’s Heartbreak</t>
+  </si>
+  <si>
+    <t>James Francies / Abigail Smith</t>
+  </si>
+  <si>
+    <t>Drake feat: YEBBA</t>
+  </si>
+  <si>
+    <t>No Friends in the Industry</t>
+  </si>
+  <si>
+    <t>Bobby DeBarge / Robert Debarge / Nik Frascona / Aubrey Graham / Anderson Hernandez / Gregory Williams / Ozan Yildirim</t>
+  </si>
+  <si>
+    <t>Knife Talk</t>
+  </si>
+  <si>
+    <t>Sheyaa Bin Abraham-Joseph / Aubrey Graham / Jordan Houston / Patrick Houston / Peter Lee Johnson / Rakim Mayers / Leland Wayne / Lil Wayne</t>
+  </si>
+  <si>
+    <t>Drake feat: Project Pat / 21 Savage</t>
+  </si>
+  <si>
+    <t>7am on Bridle Path</t>
+  </si>
+  <si>
+    <t>Maneesh Bidaye / Dylan Cleary-Krell / David Duodu / Aubrey Graham / Ronald LaTour</t>
+  </si>
+  <si>
+    <t>Race My Mind</t>
+  </si>
+  <si>
+    <t>David Axelrod / Michael Axelrod / Nile Goveia / Aubrey Graham / Osten Harvey / James Johnson / Peter Lee Johnson / Noah Shebib / Christopher Wallace / Scott Zhang</t>
+  </si>
+  <si>
+    <t>Fountains</t>
+  </si>
+  <si>
+    <t>Aubrey Graham / Temilade Openiyi / Tresor Riziki</t>
+  </si>
+  <si>
+    <t>Drake feat: Tems</t>
+  </si>
+  <si>
+    <t>Get Along Better</t>
+  </si>
+  <si>
+    <t>Noel Cadastre / Aubrey Graham / Tyrone Griffin / Paul Jefferies / Noah Shebib</t>
+  </si>
+  <si>
+    <t>Drake feat: Ty Dolla $ign</t>
+  </si>
+  <si>
+    <t>You Only Live Twice</t>
+  </si>
+  <si>
+    <t>Dwayne Carter / Aubrey Graham / Roosevelt Harrell / Brian Reid / William Roberts</t>
+  </si>
+  <si>
+    <t>Drake feat: Rick Ross / Lil Wayne</t>
+  </si>
+  <si>
+    <t>IMY2</t>
+  </si>
+  <si>
+    <t>Harley Arsenault / Dounia Aznou / Ayoub Benfaress / Eddy Bizimana / Kaniel Castaneda / Aubrey Graham / Scott Mescudi / Clifford Owuor</t>
+  </si>
+  <si>
+    <t>Drake feat: Kid Cudi</t>
+  </si>
+  <si>
+    <t>Fucking Fans</t>
+  </si>
+  <si>
+    <t>Jahron Brathwaite / Noel Cadastre / Aubrey Graham / Peter Ring / Noah Shebib</t>
+  </si>
+  <si>
+    <t>The Remorse</t>
+  </si>
+  <si>
+    <t>Aubrey Graham / Anthony Hamilton / Noah Shebib</t>
   </si>
 </sst>
 </file>
@@ -272,11 +333,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="lilnasx1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="drake8" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="lilnasx1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="drake8" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -579,15 +640,15 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
@@ -624,7 +685,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>9.5833333333333326E-2</v>
+        <v>0.23333333333333331</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -645,7 +706,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>0.15347222222222223</v>
+        <v>0.12361111111111112</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -666,7 +727,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>0.14722222222222223</v>
+        <v>0.15347222222222223</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -684,10 +745,10 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2">
-        <v>9.930555555555555E-2</v>
+        <v>0.20555555555555557</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -699,16 +760,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2">
-        <v>1.6666666666666666E-2</v>
+        <v>0.15833333333333333</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -720,16 +781,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2">
-        <v>0.12083333333333333</v>
+        <v>0.20208333333333331</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -741,16 +802,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1125</v>
+        <v>0.17847222222222223</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -762,16 +823,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.11805555555555557</v>
+        <v>0.21388888888888891</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -783,16 +844,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2">
-        <v>0.10069444444444443</v>
+        <v>0.18958333333333333</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -804,16 +865,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>0.1013888888888889</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -825,16 +886,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E12" s="2">
-        <v>0.11666666666666665</v>
+        <v>9.2361111111111116E-2</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -846,16 +907,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="5">
-        <v>0.17222222222222225</v>
+        <v>0.14166666666666666</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
@@ -867,16 +928,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E14" s="2">
-        <v>9.1666666666666674E-2</v>
+        <v>0.16874999999999998</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -888,16 +949,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="2">
-        <v>0.14652777777777778</v>
+        <v>0.16597222222222222</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -909,103 +970,187 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="E16" s="2">
-        <v>0.12708333333333333</v>
+        <v>0.18680555555555556</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="5:10">
-      <c r="E17" s="2"/>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.13333333333333333</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="5:10">
-      <c r="E18" s="2"/>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.15902777777777777</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="5:10">
-      <c r="E19" s="2"/>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.14791666666666667</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="5:10">
-      <c r="E20" s="2"/>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.17500000000000002</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="5:10">
-      <c r="E21" s="2"/>
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.17013888888888887</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="5:10">
-      <c r="E22" s="2"/>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.24374999999999999</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="5:10">
+    <row r="23" spans="1:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="5:10">
+    <row r="24" spans="1:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="5:10">
+    <row r="25" spans="1:10">
       <c r="E25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="5:10">
+    <row r="26" spans="1:10">
       <c r="E26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="5:10">
+    <row r="27" spans="1:10">
       <c r="E27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="5:10">
+    <row r="28" spans="1:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="5:10">
+    <row r="29" spans="1:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="5:10">
+    <row r="30" spans="1:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="5:10">
+    <row r="31" spans="1:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="5:10">
+    <row r="32" spans="1:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">
@@ -1022,7 +1167,7 @@
   <dimension ref="A2:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="A3:K19"/>
+      <selection activeCell="K25" sqref="A3:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -1042,11 +1187,11 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>119</v>
+        <v>263</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
@@ -1070,14 +1215,14 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                         </v>
+        <v xml:space="preserve"> Title                     </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                             </v>
+        <v xml:space="preserve"> Composers                                                                                                                                                                                                                                                             </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
@@ -1109,14 +1254,14 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------------------ </v>
+        <v xml:space="preserve">-------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
@@ -1148,28 +1293,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Montero (Call Me By Your Name)</v>
+        <v xml:space="preserve">Champagne Poetry          </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Denzel Baptiste, David Biral, Omer Fedi, Roy Lenzo, Montero Hill                                                       </v>
+        <v xml:space="preserve"> Maneesh Bidaye / Micah Davis / Aubrey Graham / Gabriel Hardeman / Jean-Andre Lawrence / John Lennon / Paul McCartney / Noah Shebib                                                                                                                                     </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X                          </v>
+        <v xml:space="preserve">Drake                              </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:18 </v>
+        <v xml:space="preserve">05:36 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1188,28 +1333,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Dead Right Now                </v>
+        <v xml:space="preserve">Papi’s Home              </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Denzel Baptiste, David Biral, Jasper Harris, Thomas James Levesque, Montero Hill                                       </v>
+        <v xml:space="preserve"> Mark Borino / Anthony "Shep" Crawford / Aubrey Graham / Raynford Humphrey / Montell Jordan / Michael Gordon Jr. / Oriyomi Ojelade / Jonathan D. Priester / Jarrel Young                                                                                                </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X                          </v>
+        <v xml:space="preserve">Drake                              </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:41 </v>
+        <v xml:space="preserve">02:58 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1228,28 +1373,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Industry Baby                 </v>
+        <v xml:space="preserve">Girls Want Girls          </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Denzel Baptiste, David Biral, Jack Harlow, Nick Lee, Montero Hill, Kanye West                                          </v>
+        <v xml:space="preserve"> Aubrey Graham / Dominique Jones / Mathias Liyew / Ozan Yildirim                                                                                                                                                                                                        </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X &amp; Jack Harlow            </v>
+        <v xml:space="preserve">Drake feat: Lil Baby               </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:32 </v>
+        <v xml:space="preserve">03:41 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1268,28 +1413,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Thats What I Want             </v>
+        <v xml:space="preserve">In the Bible              </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Omer Fedi, Keegan Bach, Montero Hill, Blake Slatkin, Ryan Tedder                                                       </v>
+        <v xml:space="preserve"> Durk Banks / Eli Brown / Eliel Brown / Giveon Evans / Simon Gebrelul / Giveon / Aubrey Graham / Leon Thomas III / Austin Schindler / Noah Shebib                                                                                                                       </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X                          </v>
+        <v xml:space="preserve">Drake feat: Lil Durk / Giveon      </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:23 </v>
+        <v xml:space="preserve">04:56 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1308,28 +1453,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">The Art of Realization        </v>
+        <v xml:space="preserve">Love All                  </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Denzel Baptiste, David Biral, Roy Lenzo, Montero Hill                                                                  </v>
+        <v xml:space="preserve"> Shawn Carter / Dylan Cleary-Krell / Luke Combs / Sean Combs / Aubrey Graham / Leon Thomas III / Majid Jordan / Steven Jordan / Khristopher Riddick-Tynes / Christopher Wallace / Ozan Yildirim                                                                         </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X                          </v>
+        <v xml:space="preserve">Drake feat: Jay-Z                  </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:24 </v>
+        <v xml:space="preserve">03:48 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1348,28 +1493,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Scoop                         </v>
+        <v xml:space="preserve">Fair Trade                </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Amala Zandile Dlamini, Denzel Baptiste, David Biral, Roy Lenzo, Montero Hill                                           </v>
+        <v xml:space="preserve"> Reibaldi Sephane Antoine / Brandon Banks / Kenneth Edmonds / Aubrey Graham / Teo Halm / Dernst Emile II / Michael Gordon Jr. / Kyla Moscovich / Ebony Oshunrinde / Marcus Reddick / Jahaan Sweet / Varren Wade / Jacques Webster / Charlotte Day Wilson / Ozan Yildirim</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X feat. Doja Cat           </v>
+        <v xml:space="preserve">Drake feat: Travis Scott           </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:54 </v>
+        <v xml:space="preserve">04:51 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1388,28 +1533,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">One of Me                     </v>
+        <v xml:space="preserve">Way 2 Sexy                </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> John Cunningham, Isley Juber, Montero Hill, Jasper Sheff                                                               </v>
+        <v xml:space="preserve"> Fred Fairbrass / Richard Fairbrass / Aubrey Graham / Rob Manzoli / Lesidney Ragland / Brandon Simmons / Bryan Simmons / Nayvadius Wilburn / Jeffery Williams                                                                                                           </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X feat. Elton John         </v>
+        <v xml:space="preserve">Drake feat: Future / Young Thug    </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:42 </v>
+        <v xml:space="preserve">04:17 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1428,28 +1573,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Lost in the Citadel           </v>
+        <v xml:space="preserve">TSU                       </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> John Cunningham, Montero Hill                                                                                          </v>
+        <v xml:space="preserve"> Harley Arsenault / Noel Cadastre / Christopher Cross / Aubrey Graham / Nate Hills / Nathaniel Hills / R. Kelly / Robert Kelly / Timothy Mosley / Justin Timberlake                                                                                                     </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X                          </v>
+        <v xml:space="preserve">Drake                              </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:50 </v>
+        <v xml:space="preserve">05:08 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1468,28 +1613,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Dolla Sign Slime              </v>
+        <v xml:space="preserve">N 2 Deep                  </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Denzel Baptiste, David Biral, Nick Lee, Megan Pete, Montero Hill                                                       </v>
+        <v xml:space="preserve"> Harley Arsenault / Kaushik Barua / Chad Butler / Noel Cadastre / Shawn Carter / B. J. Freeman / Bernard Freeman / Aubrey Graham / Jay Jenkins / Leroy Williams, Jr. / Alex Lustig / Joseph McVey / Noah Shebib / Nayvadius Wilburn / Leroy Williams                    </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Lil Nas X feat. Megan thee Stallion</v>
+        <v xml:space="preserve">Drake feat: Future                 </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:25 </v>
+        <v xml:space="preserve">04:33 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1508,28 +1653,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Tales of Dominica             </v>
+        <v xml:space="preserve">Pipe Down                 </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Denzel Baptiste, David Biral, Omer Fedi, Roy Lenzo, Montero Hill                                                       </v>
+        <v xml:space="preserve"> Lazaro Camejo / Simon Gebrelul / Aubrey Graham / Abdelhady Moamer Hafez / Leon Thomas III / Robert E. Fairfax III / Derek Kastal / Anthoine Walters / Walters                                                                                                          </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X                          </v>
+        <v xml:space="preserve">Drake                              </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:26 </v>
+        <v xml:space="preserve">03:25 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1548,28 +1693,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sun Goes Down                 </v>
+        <v xml:space="preserve">Yebba’s Heartbreak       </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Denzel Baptiste, David Biral, Omer Fedi, Keegan Bach, Roy Lenzo, Andrew Luce, Montero Hill, Michael Olmo, Blake Slatkin</v>
+        <v xml:space="preserve"> James Francies / Abigail Smith                                                                                                                                                                                                                                         </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X                          </v>
+        <v xml:space="preserve">Drake feat: YEBBA                  </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:48 </v>
+        <v xml:space="preserve">02:13 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1588,28 +1733,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Void                          </v>
+        <v>No Friends in the Industry</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> John Cunningham, Carter Lang, Montero Hill                                                                             </v>
+        <v xml:space="preserve"> Bobby DeBarge / Robert Debarge / Nik Frascona / Aubrey Graham / Anderson Hernandez / Gregory Williams / Ozan Yildirim                                                                                                                                                  </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X                          </v>
+        <v xml:space="preserve">Drake                              </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:08 </v>
+        <v xml:space="preserve">03:24 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1628,28 +1773,28 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Don't Want It                 </v>
+        <v xml:space="preserve">Knife Talk                </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Denzel Baptiste, David Biral, Nicholas Mira, Montero Hill, Dorien Theus                                                </v>
+        <v xml:space="preserve"> Sheyaa Bin Abraham-Joseph / Aubrey Graham / Jordan Houston / Patrick Houston / Peter Lee Johnson / Rakim Mayers / Leland Wayne / Lil Wayne                                                                                                                             </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X                          </v>
+        <v>Drake feat: Project Pat / 21 Savage</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:12 </v>
+        <v xml:space="preserve">04:03 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1668,28 +1813,28 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Life After Salem              </v>
+        <v xml:space="preserve">7am on Bridle Path        </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> John Cunningham, Carter Lang, Montero Hill, Jasper Sheff                                                               </v>
+        <v xml:space="preserve"> Maneesh Bidaye / Dylan Cleary-Krell / David Duodu / Aubrey Graham / Ronald LaTour                                                                                                                                                                                      </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X                          </v>
+        <v xml:space="preserve">Drake                              </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:31 </v>
+        <v xml:space="preserve">03:59 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1708,28 +1853,28 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Am I Dreaming                 </v>
+        <v xml:space="preserve">Race My Mind              </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Denzel Baptiste, David Biral, Miley Cyrus, Omer Fedi, Vincent Goodyer, Montero Hill, William K Ward                    </v>
+        <v xml:space="preserve"> David Axelrod / Michael Axelrod / Nile Goveia / Aubrey Graham / Osten Harvey / James Johnson / Peter Lee Johnson / Noah Shebib / Christopher Wallace / Scott Zhang                                                                                                     </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Lil Nas X feat. Miley Cyrus        </v>
+        <v xml:space="preserve">Drake                              </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:03 </v>
+        <v xml:space="preserve">04:29 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1741,35 +1886,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">Fountains                 </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve"> Aubrey Graham / Temilade Openiyi / Tresor Riziki                                                                                                                                                                                                                       </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">Drake feat: Tems                   </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:12 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1781,35 +1926,35 @@
       </c>
       <c r="B21">
         <f>Sheet1!A18</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">Get Along Better          </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve"> Noel Cadastre / Aubrey Graham / Tyrone Griffin / Paul Jefferies / Noah Shebib                                                                                                                                                                                          </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">Drake feat: Ty Dolla $ign          </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:49 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
@@ -1821,35 +1966,35 @@
       </c>
       <c r="B22">
         <f>Sheet1!A19</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">You Only Live Twice       </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve"> Dwayne Carter / Aubrey Graham / Roosevelt Harrell / Brian Reid / William Roberts                                                                                                                                                                                       </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">Drake feat: Rick Ross / Lil Wayne  </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="3" t="str">
         <f>TEXT(Sheet1!E19,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:33 </v>
       </c>
       <c r="K22" s="4" t="s">
         <v>0</v>
@@ -1861,35 +2006,35 @@
       </c>
       <c r="B23">
         <f>Sheet1!A20</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">IMY2                      </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve"> Harley Arsenault / Dounia Aznou / Ayoub Benfaress / Eddy Bizimana / Kaniel Castaneda / Aubrey Graham / Scott Mescudi / Clifford Owuor                                                                                                                                  </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">Drake feat: Kid Cudi               </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J23" s="3" t="str">
         <f>TEXT(Sheet1!E20,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:12 </v>
       </c>
       <c r="K23" s="4" t="s">
         <v>0</v>
@@ -1901,35 +2046,35 @@
       </c>
       <c r="B24">
         <f>Sheet1!A21</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">Fucking Fans              </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve"> Jahron Brathwaite / Noel Cadastre / Aubrey Graham / Peter Ring / Noah Shebib                                                                                                                                                                                           </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">Drake                              </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J24" s="3" t="str">
         <f>TEXT(Sheet1!E21,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:05 </v>
       </c>
       <c r="K24" s="4" t="s">
         <v>0</v>
@@ -1941,35 +2086,35 @@
       </c>
       <c r="B25">
         <f>Sheet1!A22</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">The Remorse               </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve"> Aubrey Graham / Anthony Hamilton / Noah Shebib                                                                                                                                                                                                                         </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">Drake                              </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J25" s="3" t="str">
         <f>TEXT(Sheet1!E22,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">05:51 </v>
       </c>
       <c r="K25" s="4" t="s">
         <v>0</v>
@@ -1988,14 +2133,14 @@
       </c>
       <c r="D26" t="str">
         <f>LEFTB(Sheet1!B23&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="str">
         <f>" "&amp;LEFTB(Sheet1!C23&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
       </c>
       <c r="G26" s="4" t="s">
         <v>0</v>
@@ -2028,14 +2173,14 @@
       </c>
       <c r="D27" t="str">
         <f>LEFTB(Sheet1!B24&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="str">
         <f>" "&amp;LEFTB(Sheet1!C24&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
       </c>
       <c r="G27" s="4" t="s">
         <v>0</v>
@@ -2068,14 +2213,14 @@
       </c>
       <c r="D28" t="str">
         <f>LEFTB(Sheet1!B25&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F28" t="str">
         <f>" "&amp;LEFTB(Sheet1!C25&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
       </c>
       <c r="G28" s="4" t="s">
         <v>0</v>
@@ -2108,14 +2253,14 @@
       </c>
       <c r="D29" t="str">
         <f>LEFTB(Sheet1!B26&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E29" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F29" t="str">
         <f>" "&amp;LEFTB(Sheet1!C26&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
       </c>
       <c r="G29" s="4" t="s">
         <v>0</v>
@@ -2148,14 +2293,14 @@
       </c>
       <c r="D30" t="str">
         <f>LEFTB(Sheet1!B27&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F30" t="str">
         <f>" "&amp;LEFTB(Sheet1!C27&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
       </c>
       <c r="G30" s="4" t="s">
         <v>0</v>
@@ -2188,14 +2333,14 @@
       </c>
       <c r="D31" t="str">
         <f>LEFTB(Sheet1!B28&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F31" t="str">
         <f>" "&amp;LEFTB(Sheet1!C28&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
       </c>
       <c r="G31" s="4" t="s">
         <v>0</v>
@@ -2228,14 +2373,14 @@
       </c>
       <c r="D32" t="str">
         <f>LEFTB(Sheet1!B29&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F32" t="str">
         <f>" "&amp;LEFTB(Sheet1!C29&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
       </c>
       <c r="G32" s="4" t="s">
         <v>0</v>
@@ -2268,14 +2413,14 @@
       </c>
       <c r="D33" t="str">
         <f>LEFTB(Sheet1!B30&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F33" t="str">
         <f>" "&amp;LEFTB(Sheet1!C30&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
       </c>
       <c r="G33" s="4" t="s">
         <v>0</v>
@@ -2313,9 +2458,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
@@ -2352,7 +2497,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>9.5833333333333326E-2</v>
+        <v>0.23333333333333331</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2373,7 +2518,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>0.15347222222222223</v>
+        <v>0.12361111111111112</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2394,7 +2539,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>0.14722222222222223</v>
+        <v>0.15347222222222223</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2412,10 +2557,10 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2">
-        <v>9.930555555555555E-2</v>
+        <v>0.20555555555555557</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2427,16 +2572,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2">
-        <v>1.6666666666666666E-2</v>
+        <v>0.15833333333333333</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2448,16 +2593,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2">
-        <v>0.12083333333333333</v>
+        <v>0.20208333333333331</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2469,16 +2614,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1125</v>
+        <v>0.17847222222222223</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2490,16 +2635,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.11805555555555557</v>
+        <v>0.21388888888888891</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2511,16 +2656,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2">
-        <v>0.10069444444444443</v>
+        <v>0.18958333333333333</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2532,16 +2677,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>0.1013888888888889</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2553,16 +2698,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E12" s="2">
-        <v>0.11666666666666665</v>
+        <v>9.2361111111111116E-2</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2574,16 +2719,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="5">
-        <v>0.17222222222222225</v>
+        <v>0.14166666666666666</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
@@ -2595,16 +2740,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E14" s="2">
-        <v>9.1666666666666674E-2</v>
+        <v>0.16874999999999998</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2616,16 +2761,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="2">
-        <v>0.14652777777777778</v>
+        <v>0.16597222222222222</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -2637,103 +2782,187 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="E16" s="2">
-        <v>0.12708333333333333</v>
+        <v>0.18680555555555556</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="5:10">
-      <c r="E17" s="2"/>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.13333333333333333</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="5:10">
-      <c r="E18" s="2"/>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.15902777777777777</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="5:10">
-      <c r="E19" s="2"/>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.14791666666666667</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="5:10">
-      <c r="E20" s="2"/>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.17500000000000002</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="5:10">
-      <c r="E21" s="2"/>
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.17013888888888887</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="5:10">
-      <c r="E22" s="2"/>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.24374999999999999</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="5:10">
+    <row r="23" spans="1:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="5:10">
+    <row r="24" spans="1:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="5:10">
+    <row r="25" spans="1:10">
       <c r="E25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="5:10">
+    <row r="26" spans="1:10">
       <c r="E26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="5:10">
+    <row r="27" spans="1:10">
       <c r="E27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="5:10">
+    <row r="28" spans="1:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="5:10">
+    <row r="29" spans="1:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="5:10">
+    <row r="30" spans="1:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="5:10">
+    <row r="31" spans="1:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="5:10">
+    <row r="32" spans="1:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">

</xml_diff>

<commit_message>
01172000 added rev ss
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,11 +17,10 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="drake8" localSheetId="0">Sheet1!$A$1:$E$22</definedName>
-    <definedName name="drake8" localSheetId="2">Sheet3!$A$1:$E$22</definedName>
+    <definedName name="silksonic1" localSheetId="0">Sheet1!$A$1:$E$10</definedName>
+    <definedName name="silksonic1" localSheetId="2">Sheet3!$A$1:$E$10</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/drake8.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/silksonic1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/drake8.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/silksonic1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="23">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -76,169 +75,52 @@
     <t>Composer</t>
   </si>
   <si>
-    <t>Champagne Poetry</t>
+    <t>Silk Sonic Intro</t>
   </si>
   <si>
-    <t>Maneesh Bidaye / Micah Davis / Aubrey Graham / Gabriel Hardeman / Jean-Andre Lawrence / John Lennon / Paul McCartney / Noah Shebib</t>
+    <t>Bruno Mars, Brandon Anderson, Dernst Emile II</t>
   </si>
   <si>
-    <t>Drake</t>
+    <t>Silk Sonic</t>
   </si>
   <si>
-    <t>Papi’s Home</t>
+    <t>Leave the Door Open</t>
   </si>
   <si>
-    <t>Mark Borino / Anthony "Shep" Crawford / Aubrey Graham / Raynford Humphrey / Montell Jordan / Michael Gordon Jr. / Oriyomi Ojelade / Jonathan D. Priester / Jarrel Young</t>
+    <t>Bruno Mars, Brandon Anderson, Dernst Emile II, Christopher Brody Brown</t>
   </si>
   <si>
-    <t>Girls Want Girls</t>
+    <t>Fly as Me</t>
   </si>
   <si>
-    <t>Aubrey Graham / Dominique Jones / Mathias Liyew / Ozan Yildirim</t>
+    <t>Bruno Mars, Brandon Anderson, Dernst Emile II, James Fauntleroy, Span Anderson</t>
   </si>
   <si>
-    <t>Drake feat: Lil Baby</t>
+    <t>After Last Night</t>
   </si>
   <si>
-    <t>In the Bible</t>
+    <t>Bruno Mars, Brandon Anderson, Dernst Emile II, James Fauntleroy, Stephen Bruner, Jonathan Yip, Ray Ronulas, Jeremy Reeves, Ray Charles McCullough II</t>
   </si>
   <si>
-    <t>Durk Banks / Eli Brown / Eliel Brown / Giveon Evans / Simon Gebrelul / Giveon / Aubrey Graham / Leon Thomas III / Austin Schindler / Noah Shebib</t>
+    <t>Silk Sonic w/ Thundercat and Booty</t>
   </si>
   <si>
-    <t>Drake feat: Lil Durk / Giveon</t>
+    <t>Smokin Out the Window</t>
   </si>
   <si>
-    <t>Love All</t>
+    <t>Put on a Smile</t>
   </si>
   <si>
-    <t>Shawn Carter / Dylan Cleary-Krell / Luke Combs / Sean Combs / Aubrey Graham / Leon Thomas III / Majid Jordan / Steven Jordan / Khristopher Riddick-Tynes / Christopher Wallace / Ozan Yildirim</t>
+    <t>Bruno Mars, Brandon Anderson, Dernst Emile II, Kenny "Babyface" Edmonds</t>
   </si>
   <si>
-    <t>Drake feat: Jay-Z</t>
+    <t>Skate</t>
   </si>
   <si>
-    <t>Fair Trade</t>
+    <t>Bruno Mars, Brandon Anderson, Dernst Emile II, James Fauntleroy, Domitille Degalle, J. D. Beck</t>
   </si>
   <si>
-    <t>Reibaldi Sephane Antoine / Brandon Banks / Kenneth Edmonds / Aubrey Graham / Teo Halm / Dernst Emile II / Michael Gordon Jr. / Kyla Moscovich / Ebony Oshunrinde / Marcus Reddick / Jahaan Sweet / Varren Wade / Jacques Webster / Charlotte Day Wilson / Ozan Yildirim</t>
-  </si>
-  <si>
-    <t>Drake feat: Travis Scott</t>
-  </si>
-  <si>
-    <t>Way 2 Sexy</t>
-  </si>
-  <si>
-    <t>Fred Fairbrass / Richard Fairbrass / Aubrey Graham / Rob Manzoli / Lesidney Ragland / Brandon Simmons / Bryan Simmons / Nayvadius Wilburn / Jeffery Williams</t>
-  </si>
-  <si>
-    <t>Drake feat: Future / Young Thug</t>
-  </si>
-  <si>
-    <t>TSU</t>
-  </si>
-  <si>
-    <t>Harley Arsenault / Noel Cadastre / Christopher Cross / Aubrey Graham / Nate Hills / Nathaniel Hills / R. Kelly / Robert Kelly / Timothy Mosley / Justin Timberlake</t>
-  </si>
-  <si>
-    <t>N 2 Deep</t>
-  </si>
-  <si>
-    <t>Harley Arsenault / Kaushik Barua / Chad Butler / Noel Cadastre / Shawn Carter / B. J. Freeman / Bernard Freeman / Aubrey Graham / Jay Jenkins / Leroy Williams, Jr. / Alex Lustig / Joseph McVey / Noah Shebib / Nayvadius Wilburn / Leroy Williams</t>
-  </si>
-  <si>
-    <t>Drake feat: Future</t>
-  </si>
-  <si>
-    <t>Pipe Down</t>
-  </si>
-  <si>
-    <t>Lazaro Camejo / Simon Gebrelul / Aubrey Graham / Abdelhady Moamer Hafez / Leon Thomas III / Robert E. Fairfax III / Derek Kastal / Anthoine Walters / Walters</t>
-  </si>
-  <si>
-    <t>Yebba’s Heartbreak</t>
-  </si>
-  <si>
-    <t>James Francies / Abigail Smith</t>
-  </si>
-  <si>
-    <t>Drake feat: YEBBA</t>
-  </si>
-  <si>
-    <t>No Friends in the Industry</t>
-  </si>
-  <si>
-    <t>Bobby DeBarge / Robert Debarge / Nik Frascona / Aubrey Graham / Anderson Hernandez / Gregory Williams / Ozan Yildirim</t>
-  </si>
-  <si>
-    <t>Knife Talk</t>
-  </si>
-  <si>
-    <t>Sheyaa Bin Abraham-Joseph / Aubrey Graham / Jordan Houston / Patrick Houston / Peter Lee Johnson / Rakim Mayers / Leland Wayne / Lil Wayne</t>
-  </si>
-  <si>
-    <t>Drake feat: Project Pat / 21 Savage</t>
-  </si>
-  <si>
-    <t>7am on Bridle Path</t>
-  </si>
-  <si>
-    <t>Maneesh Bidaye / Dylan Cleary-Krell / David Duodu / Aubrey Graham / Ronald LaTour</t>
-  </si>
-  <si>
-    <t>Race My Mind</t>
-  </si>
-  <si>
-    <t>David Axelrod / Michael Axelrod / Nile Goveia / Aubrey Graham / Osten Harvey / James Johnson / Peter Lee Johnson / Noah Shebib / Christopher Wallace / Scott Zhang</t>
-  </si>
-  <si>
-    <t>Fountains</t>
-  </si>
-  <si>
-    <t>Aubrey Graham / Temilade Openiyi / Tresor Riziki</t>
-  </si>
-  <si>
-    <t>Drake feat: Tems</t>
-  </si>
-  <si>
-    <t>Get Along Better</t>
-  </si>
-  <si>
-    <t>Noel Cadastre / Aubrey Graham / Tyrone Griffin / Paul Jefferies / Noah Shebib</t>
-  </si>
-  <si>
-    <t>Drake feat: Ty Dolla $ign</t>
-  </si>
-  <si>
-    <t>You Only Live Twice</t>
-  </si>
-  <si>
-    <t>Dwayne Carter / Aubrey Graham / Roosevelt Harrell / Brian Reid / William Roberts</t>
-  </si>
-  <si>
-    <t>Drake feat: Rick Ross / Lil Wayne</t>
-  </si>
-  <si>
-    <t>IMY2</t>
-  </si>
-  <si>
-    <t>Harley Arsenault / Dounia Aznou / Ayoub Benfaress / Eddy Bizimana / Kaniel Castaneda / Aubrey Graham / Scott Mescudi / Clifford Owuor</t>
-  </si>
-  <si>
-    <t>Drake feat: Kid Cudi</t>
-  </si>
-  <si>
-    <t>Fucking Fans</t>
-  </si>
-  <si>
-    <t>Jahron Brathwaite / Noel Cadastre / Aubrey Graham / Peter Ring / Noah Shebib</t>
-  </si>
-  <si>
-    <t>The Remorse</t>
-  </si>
-  <si>
-    <t>Aubrey Graham / Anthony Hamilton / Noah Shebib</t>
+    <t>Blast Off</t>
   </si>
 </sst>
 </file>
@@ -333,11 +215,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="drake8" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="silksonic1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="drake8" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="silksonic1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -640,16 +522,16 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="24.21875" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
@@ -685,7 +567,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.23333333333333331</v>
+        <v>4.3750000000000004E-2</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -706,7 +588,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>0.12361111111111112</v>
+        <v>0.16805555555555554</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -724,10 +606,10 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15347222222222223</v>
+        <v>0.15208333333333332</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -739,16 +621,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" s="2">
-        <v>0.20555555555555557</v>
+        <v>0.17291666666666669</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -760,16 +642,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>0.15833333333333333</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -781,16 +663,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>0.20208333333333331</v>
+        <v>0.17708333333333334</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -801,17 +683,17 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
+      <c r="B8">
+        <v>777</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2">
-        <v>0.17847222222222223</v>
+        <v>0.11388888888888889</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -823,16 +705,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.21388888888888891</v>
+        <v>0.14097222222222222</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -844,16 +726,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>0.18958333333333333</v>
+        <v>0.19722222222222222</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -861,296 +743,130 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.1423611111111111</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="2">
-        <v>9.2361111111111116E-2</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.14166666666666666</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.16874999999999998</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.16597222222222222</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.18680555555555556</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.13333333333333333</v>
-      </c>
+    <row r="17" spans="5:10">
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.15902777777777777</v>
-      </c>
+    <row r="18" spans="5:10">
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.14791666666666667</v>
-      </c>
+    <row r="19" spans="5:10">
+      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.17500000000000002</v>
-      </c>
+    <row r="20" spans="5:10">
+      <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.17013888888888887</v>
-      </c>
+    <row r="21" spans="5:10">
+      <c r="E21" s="2"/>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.24374999999999999</v>
-      </c>
+    <row r="22" spans="5:10">
+      <c r="E22" s="2"/>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="5:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="5:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="5:10">
       <c r="E25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="5:10">
       <c r="E26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="5:10">
       <c r="E27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="5:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="5:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="5:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="5:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="5:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">
@@ -1167,7 +883,7 @@
   <dimension ref="A2:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="A3:K25"/>
+      <selection activeCell="K13" sqref="A3:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -1187,15 +903,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>263</v>
+        <v>148</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -1215,21 +931,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                     </v>
+        <v xml:space="preserve"> Title                </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                                                                                                                                             </v>
+        <v xml:space="preserve"> Composers                                                                                                                                          </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                          </v>
+        <v xml:space="preserve"> Performer                         </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1254,21 +970,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">-------------------------- </v>
+        <v xml:space="preserve">--------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ---------------------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------- </v>
+        <v xml:space="preserve"> ---------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1293,28 +1009,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Champagne Poetry          </v>
+        <v xml:space="preserve">Silk Sonic Intro     </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Maneesh Bidaye / Micah Davis / Aubrey Graham / Gabriel Hardeman / Jean-Andre Lawrence / John Lennon / Paul McCartney / Noah Shebib                                                                                                                                     </v>
+        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II                                                                                                       </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake                              </v>
+        <v xml:space="preserve">Silk Sonic                        </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:36 </v>
+        <v xml:space="preserve">01:03 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1333,28 +1049,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Papi’s Home              </v>
+        <v xml:space="preserve">Leave the Door Open  </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Mark Borino / Anthony "Shep" Crawford / Aubrey Graham / Raynford Humphrey / Montell Jordan / Michael Gordon Jr. / Oriyomi Ojelade / Jonathan D. Priester / Jarrel Young                                                                                                </v>
+        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II, Christopher Brody Brown                                                                              </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake                              </v>
+        <v xml:space="preserve">Silk Sonic                        </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:58 </v>
+        <v xml:space="preserve">04:02 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1373,28 +1089,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Girls Want Girls          </v>
+        <v xml:space="preserve">Fly as Me            </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aubrey Graham / Dominique Jones / Mathias Liyew / Ozan Yildirim                                                                                                                                                                                                        </v>
+        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II, James Fauntleroy, Span Anderson                                                                      </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake feat: Lil Baby               </v>
+        <v xml:space="preserve">Silk Sonic                        </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:41 </v>
+        <v xml:space="preserve">03:39 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1413,28 +1129,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">In the Bible              </v>
+        <v xml:space="preserve">After Last Night     </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Durk Banks / Eli Brown / Eliel Brown / Giveon Evans / Simon Gebrelul / Giveon / Aubrey Graham / Leon Thomas III / Austin Schindler / Noah Shebib                                                                                                                       </v>
+        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II, James Fauntleroy, Stephen Bruner, Jonathan Yip, Ray Ronulas, Jeremy Reeves, Ray Charles McCullough II</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake feat: Lil Durk / Giveon      </v>
+        <v>Silk Sonic w/ Thundercat and Booty</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:56 </v>
+        <v xml:space="preserve">04:09 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1453,28 +1169,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Love All                  </v>
+        <v>Smokin Out the Window</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Shawn Carter / Dylan Cleary-Krell / Luke Combs / Sean Combs / Aubrey Graham / Leon Thomas III / Majid Jordan / Steven Jordan / Khristopher Riddick-Tynes / Christopher Wallace / Ozan Yildirim                                                                         </v>
+        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II                                                                                                       </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake feat: Jay-Z                  </v>
+        <v xml:space="preserve">Silk Sonic                        </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:48 </v>
+        <v xml:space="preserve">03:17 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1493,28 +1209,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Fair Trade                </v>
+        <v xml:space="preserve">Put on a Smile       </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Reibaldi Sephane Antoine / Brandon Banks / Kenneth Edmonds / Aubrey Graham / Teo Halm / Dernst Emile II / Michael Gordon Jr. / Kyla Moscovich / Ebony Oshunrinde / Marcus Reddick / Jahaan Sweet / Varren Wade / Jacques Webster / Charlotte Day Wilson / Ozan Yildirim</v>
+        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II, Kenny "Babyface" Edmonds                                                                             </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake feat: Travis Scott           </v>
+        <v xml:space="preserve">Silk Sonic                        </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:51 </v>
+        <v xml:space="preserve">04:15 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1533,28 +1249,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Way 2 Sexy                </v>
+        <v xml:space="preserve">777                  </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Fred Fairbrass / Richard Fairbrass / Aubrey Graham / Rob Manzoli / Lesidney Ragland / Brandon Simmons / Bryan Simmons / Nayvadius Wilburn / Jeffery Williams                                                                                                           </v>
+        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II, Christopher Brody Brown                                                                              </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake feat: Future / Young Thug    </v>
+        <v xml:space="preserve">Silk Sonic                        </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:17 </v>
+        <v xml:space="preserve">02:44 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1573,28 +1289,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">TSU                       </v>
+        <v xml:space="preserve">Skate                </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Harley Arsenault / Noel Cadastre / Christopher Cross / Aubrey Graham / Nate Hills / Nathaniel Hills / R. Kelly / Robert Kelly / Timothy Mosley / Justin Timberlake                                                                                                     </v>
+        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II, James Fauntleroy, Domitille Degalle, J. D. Beck                                                      </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake                              </v>
+        <v xml:space="preserve">Silk Sonic                        </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:08 </v>
+        <v xml:space="preserve">03:23 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1613,28 +1329,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">N 2 Deep                  </v>
+        <v xml:space="preserve">Blast Off            </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Harley Arsenault / Kaushik Barua / Chad Butler / Noel Cadastre / Shawn Carter / B. J. Freeman / Bernard Freeman / Aubrey Graham / Jay Jenkins / Leroy Williams, Jr. / Alex Lustig / Joseph McVey / Noah Shebib / Nayvadius Wilburn / Leroy Williams                    </v>
+        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II                                                                                                       </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake feat: Future                 </v>
+        <v xml:space="preserve">Silk Sonic                        </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:33 </v>
+        <v xml:space="preserve">04:44 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1646,35 +1362,35 @@
       </c>
       <c r="B14">
         <f>Sheet1!A11</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Pipe Down                 </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Lazaro Camejo / Simon Gebrelul / Aubrey Graham / Abdelhady Moamer Hafez / Leon Thomas III / Robert E. Fairfax III / Derek Kastal / Anthoine Walters / Walters                                                                                                          </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake                              </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:25 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1686,35 +1402,35 @@
       </c>
       <c r="B15">
         <f>Sheet1!A12</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Yebba’s Heartbreak       </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> James Francies / Abigail Smith                                                                                                                                                                                                                                         </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake feat: YEBBA                  </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:13 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1726,35 +1442,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>No Friends in the Industry</v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Bobby DeBarge / Robert Debarge / Nik Frascona / Aubrey Graham / Anderson Hernandez / Gregory Williams / Ozan Yildirim                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake                              </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:24 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1766,35 +1482,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Knife Talk                </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Sheyaa Bin Abraham-Joseph / Aubrey Graham / Jordan Houston / Patrick Houston / Peter Lee Johnson / Rakim Mayers / Leland Wayne / Lil Wayne                                                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Drake feat: Project Pat / 21 Savage</v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:03 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1806,35 +1522,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">7am on Bridle Path        </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Maneesh Bidaye / Dylan Cleary-Krell / David Duodu / Aubrey Graham / Ronald LaTour                                                                                                                                                                                      </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake                              </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:59 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1846,35 +1562,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Race My Mind              </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> David Axelrod / Michael Axelrod / Nile Goveia / Aubrey Graham / Osten Harvey / James Johnson / Peter Lee Johnson / Noah Shebib / Christopher Wallace / Scott Zhang                                                                                                     </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake                              </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:29 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1886,35 +1602,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Fountains                 </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aubrey Graham / Temilade Openiyi / Tresor Riziki                                                                                                                                                                                                                       </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake feat: Tems                   </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:12 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1926,35 +1642,35 @@
       </c>
       <c r="B21">
         <f>Sheet1!A18</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Get Along Better          </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Noel Cadastre / Aubrey Graham / Tyrone Griffin / Paul Jefferies / Noah Shebib                                                                                                                                                                                          </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake feat: Ty Dolla $ign          </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:49 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
@@ -1966,35 +1682,35 @@
       </c>
       <c r="B22">
         <f>Sheet1!A19</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">You Only Live Twice       </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dwayne Carter / Aubrey Graham / Roosevelt Harrell / Brian Reid / William Roberts                                                                                                                                                                                       </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake feat: Rick Ross / Lil Wayne  </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="3" t="str">
         <f>TEXT(Sheet1!E19,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:33 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K22" s="4" t="s">
         <v>0</v>
@@ -2006,35 +1722,35 @@
       </c>
       <c r="B23">
         <f>Sheet1!A20</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">IMY2                      </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Harley Arsenault / Dounia Aznou / Ayoub Benfaress / Eddy Bizimana / Kaniel Castaneda / Aubrey Graham / Scott Mescudi / Clifford Owuor                                                                                                                                  </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake feat: Kid Cudi               </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J23" s="3" t="str">
         <f>TEXT(Sheet1!E20,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:12 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K23" s="4" t="s">
         <v>0</v>
@@ -2046,35 +1762,35 @@
       </c>
       <c r="B24">
         <f>Sheet1!A21</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Fucking Fans              </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jahron Brathwaite / Noel Cadastre / Aubrey Graham / Peter Ring / Noah Shebib                                                                                                                                                                                           </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake                              </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J24" s="3" t="str">
         <f>TEXT(Sheet1!E21,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:05 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K24" s="4" t="s">
         <v>0</v>
@@ -2086,35 +1802,35 @@
       </c>
       <c r="B25">
         <f>Sheet1!A22</f>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">The Remorse               </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Aubrey Graham / Anthony Hamilton / Noah Shebib                                                                                                                                                                                                                         </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Drake                              </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J25" s="3" t="str">
         <f>TEXT(Sheet1!E22,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:51 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K25" s="4" t="s">
         <v>0</v>
@@ -2133,21 +1849,21 @@
       </c>
       <c r="D26" t="str">
         <f>LEFTB(Sheet1!B23&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="str">
         <f>" "&amp;LEFTB(Sheet1!C23&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H26" t="str">
         <f>LEFTB(Sheet1!D23&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I26" s="4" t="s">
         <v>0</v>
@@ -2173,21 +1889,21 @@
       </c>
       <c r="D27" t="str">
         <f>LEFTB(Sheet1!B24&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="str">
         <f>" "&amp;LEFTB(Sheet1!C24&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H27" t="str">
         <f>LEFTB(Sheet1!D24&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I27" s="4" t="s">
         <v>0</v>
@@ -2213,21 +1929,21 @@
       </c>
       <c r="D28" t="str">
         <f>LEFTB(Sheet1!B25&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F28" t="str">
         <f>" "&amp;LEFTB(Sheet1!C25&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H28" t="str">
         <f>LEFTB(Sheet1!D25&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I28" s="4" t="s">
         <v>0</v>
@@ -2253,21 +1969,21 @@
       </c>
       <c r="D29" t="str">
         <f>LEFTB(Sheet1!B26&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E29" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F29" t="str">
         <f>" "&amp;LEFTB(Sheet1!C26&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G29" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H29" t="str">
         <f>LEFTB(Sheet1!D26&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I29" s="4" t="s">
         <v>0</v>
@@ -2293,21 +2009,21 @@
       </c>
       <c r="D30" t="str">
         <f>LEFTB(Sheet1!B27&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F30" t="str">
         <f>" "&amp;LEFTB(Sheet1!C27&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H30" t="str">
         <f>LEFTB(Sheet1!D27&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I30" s="4" t="s">
         <v>0</v>
@@ -2333,21 +2049,21 @@
       </c>
       <c r="D31" t="str">
         <f>LEFTB(Sheet1!B28&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F31" t="str">
         <f>" "&amp;LEFTB(Sheet1!C28&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H31" t="str">
         <f>LEFTB(Sheet1!D28&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I31" s="4" t="s">
         <v>0</v>
@@ -2373,21 +2089,21 @@
       </c>
       <c r="D32" t="str">
         <f>LEFTB(Sheet1!B29&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F32" t="str">
         <f>" "&amp;LEFTB(Sheet1!C29&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H32" t="str">
         <f>LEFTB(Sheet1!D29&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I32" s="4" t="s">
         <v>0</v>
@@ -2413,21 +2129,21 @@
       </c>
       <c r="D33" t="str">
         <f>LEFTB(Sheet1!B30&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F33" t="str">
         <f>" "&amp;LEFTB(Sheet1!C30&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H33" t="str">
         <f>LEFTB(Sheet1!D30&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I33" s="4" t="s">
         <v>0</v>
@@ -2457,11 +2173,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="24.21875" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
@@ -2497,7 +2213,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.23333333333333331</v>
+        <v>4.3750000000000004E-2</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2518,7 +2234,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>0.12361111111111112</v>
+        <v>0.16805555555555554</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2536,10 +2252,10 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15347222222222223</v>
+        <v>0.15208333333333332</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2551,16 +2267,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" s="2">
-        <v>0.20555555555555557</v>
+        <v>0.17291666666666669</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2572,16 +2288,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>0.15833333333333333</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2593,16 +2309,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>0.20208333333333331</v>
+        <v>0.17708333333333334</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2613,17 +2329,17 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
+      <c r="B8">
+        <v>777</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2">
-        <v>0.17847222222222223</v>
+        <v>0.11388888888888889</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2635,16 +2351,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.21388888888888891</v>
+        <v>0.14097222222222222</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2656,16 +2372,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>0.18958333333333333</v>
+        <v>0.19722222222222222</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2673,296 +2389,130 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.1423611111111111</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="2">
-        <v>9.2361111111111116E-2</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.14166666666666666</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.16874999999999998</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.16597222222222222</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.18680555555555556</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.13333333333333333</v>
-      </c>
+    <row r="17" spans="5:10">
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.15902777777777777</v>
-      </c>
+    <row r="18" spans="5:10">
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.14791666666666667</v>
-      </c>
+    <row r="19" spans="5:10">
+      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.17500000000000002</v>
-      </c>
+    <row r="20" spans="5:10">
+      <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.17013888888888887</v>
-      </c>
+    <row r="21" spans="5:10">
+      <c r="E21" s="2"/>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.24374999999999999</v>
-      </c>
+    <row r="22" spans="5:10">
+      <c r="E22" s="2"/>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="5:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="5:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="5:10">
       <c r="E25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="5:10">
       <c r="E26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="5:10">
       <c r="E27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="5:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="5:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="5:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="5:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="5:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">

</xml_diff>

<commit_message>
01242139 added rev mh
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="silksonic1" localSheetId="0">Sheet1!$A$1:$E$10</definedName>
-    <definedName name="silksonic1" localSheetId="2">Sheet3!$A$1:$E$10</definedName>
+    <definedName name="machhommy1" localSheetId="0">Sheet1!$A$1:$E$17</definedName>
+    <definedName name="machhommy1" localSheetId="2">Sheet3!$A$1:$E$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/silksonic1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/machhommy1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/silksonic1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/machhommy1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="29">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -75,52 +75,70 @@
     <t>Composer</t>
   </si>
   <si>
-    <t>Silk Sonic Intro</t>
-  </si>
-  <si>
-    <t>Bruno Mars, Brandon Anderson, Dernst Emile II</t>
-  </si>
-  <si>
-    <t>Silk Sonic</t>
-  </si>
-  <si>
-    <t>Leave the Door Open</t>
-  </si>
-  <si>
-    <t>Bruno Mars, Brandon Anderson, Dernst Emile II, Christopher Brody Brown</t>
-  </si>
-  <si>
-    <t>Fly as Me</t>
-  </si>
-  <si>
-    <t>Bruno Mars, Brandon Anderson, Dernst Emile II, James Fauntleroy, Span Anderson</t>
-  </si>
-  <si>
-    <t>After Last Night</t>
-  </si>
-  <si>
-    <t>Bruno Mars, Brandon Anderson, Dernst Emile II, James Fauntleroy, Stephen Bruner, Jonathan Yip, Ray Ronulas, Jeremy Reeves, Ray Charles McCullough II</t>
-  </si>
-  <si>
-    <t>Silk Sonic w/ Thundercat and Booty</t>
-  </si>
-  <si>
-    <t>Smokin Out the Window</t>
-  </si>
-  <si>
-    <t>Put on a Smile</t>
-  </si>
-  <si>
-    <t>Bruno Mars, Brandon Anderson, Dernst Emile II, Kenny "Babyface" Edmonds</t>
-  </si>
-  <si>
-    <t>Skate</t>
-  </si>
-  <si>
-    <t>Bruno Mars, Brandon Anderson, Dernst Emile II, James Fauntleroy, Domitille Degalle, J. D. Beck</t>
-  </si>
-  <si>
-    <t>Blast Off</t>
+    <t>The 26th Letter</t>
+  </si>
+  <si>
+    <t>Mach-Hommy</t>
+  </si>
+  <si>
+    <t>No Blood No Sweat</t>
+  </si>
+  <si>
+    <t>Folie Á Deux</t>
+  </si>
+  <si>
+    <t>Mach-Hommy feat. Keisha Plum, Westside Gunn</t>
+  </si>
+  <si>
+    <t>Makrel Jaxon</t>
+  </si>
+  <si>
+    <t>The Stellar Ray Theory</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>Leta Yo (Skit)</t>
+  </si>
+  <si>
+    <t>Kriminel</t>
+  </si>
+  <si>
+    <t>Pen Rale</t>
+  </si>
+  <si>
+    <t>Murder Czn</t>
+  </si>
+  <si>
+    <t>Mach-Hommy feat. Westside Gunn</t>
+  </si>
+  <si>
+    <t>Magnum Band</t>
+  </si>
+  <si>
+    <t>Mach-Hommy feat. ThaGodFahim</t>
+  </si>
+  <si>
+    <t>Rami</t>
+  </si>
+  <si>
+    <t>Kreyol (Skit)</t>
+  </si>
+  <si>
+    <t>Au Revoir</t>
+  </si>
+  <si>
+    <t>Mach-Hommy feat. Melanie Charles</t>
+  </si>
+  <si>
+    <t>Blockchain</t>
+  </si>
+  <si>
+    <t>Ten Boxes / Sin Eater</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2:50</t>
   </si>
 </sst>
 </file>
@@ -215,11 +233,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="silksonic1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="machhommy1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="silksonic1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="machhommy1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,11 +545,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="45" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
@@ -560,14 +578,11 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="2">
-        <v>4.3750000000000004E-2</v>
+        <v>0.15208333333333332</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -579,16 +594,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.16805555555555554</v>
+        <v>7.9166666666666663E-2</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -600,16 +612,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15208333333333332</v>
+        <v>0.1076388888888889</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -621,16 +630,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.17291666666666669</v>
+        <v>8.4027777777777771E-2</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -642,16 +648,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
       <c r="E6" s="2">
-        <v>0.13680555555555554</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -663,16 +667,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.17708333333333334</v>
+        <v>0.1173611111111111</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -683,17 +684,14 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>777</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
+      <c r="B8" t="s">
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.11388888888888889</v>
+        <v>2.361111111111111E-2</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -705,16 +703,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.14097222222222222</v>
+        <v>0.10833333333333334</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -726,16 +721,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
       <c r="E10" s="2">
-        <v>0.19722222222222222</v>
+        <v>7.013888888888889E-2</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -743,57 +735,133 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="E11" s="2"/>
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.14444444444444446</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="E12" s="2"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.11597222222222221</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="B13" s="5"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="C13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.10277777777777779</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4.5833333333333337E-2</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.15833333333333333</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="E16" s="2"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2">
+        <v>7.4305555555555555E-2</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="5:10">
-      <c r="E17" s="2"/>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="5:10">
+    <row r="18" spans="1:10">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -801,7 +869,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="5:10">
+    <row r="19" spans="1:10">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -809,64 +877,64 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="5:10">
+    <row r="20" spans="1:10">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="5:10">
+    <row r="21" spans="1:10">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="5:10">
+    <row r="22" spans="1:10">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="5:10">
+    <row r="23" spans="1:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="5:10">
+    <row r="24" spans="1:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="5:10">
+    <row r="25" spans="1:10">
       <c r="E25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="5:10">
+    <row r="26" spans="1:10">
       <c r="E26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="5:10">
+    <row r="27" spans="1:10">
       <c r="E27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="5:10">
+    <row r="28" spans="1:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="5:10">
+    <row r="29" spans="1:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="5:10">
+    <row r="30" spans="1:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="5:10">
+    <row r="31" spans="1:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="5:10">
+    <row r="32" spans="1:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">
@@ -883,7 +951,7 @@
   <dimension ref="A2:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="A3:K13"/>
+      <selection activeCell="K20" sqref="A3:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -903,15 +971,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>148</v>
+        <v>8</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -931,21 +999,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                </v>
+        <v xml:space="preserve"> Title                 </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                          </v>
+        <v xml:space="preserve"> Compose</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                         </v>
+        <v xml:space="preserve"> Performer                                  </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -970,21 +1038,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">--------------------- </v>
+        <v xml:space="preserve">---------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> -------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1009,28 +1077,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Silk Sonic Intro     </v>
+        <v xml:space="preserve">The 26th Letter       </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II                                                                                                       </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Silk Sonic                        </v>
+        <v xml:space="preserve">Mach-Hommy                                 </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:03 </v>
+        <v xml:space="preserve">03:39 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1049,28 +1117,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Leave the Door Open  </v>
+        <v xml:space="preserve">No Blood No Sweat     </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II, Christopher Brody Brown                                                                              </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Silk Sonic                        </v>
+        <v xml:space="preserve">Mach-Hommy                                 </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:02 </v>
+        <v xml:space="preserve">01:54 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1089,28 +1157,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Fly as Me            </v>
+        <v xml:space="preserve">Folie Á Deux         </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II, James Fauntleroy, Span Anderson                                                                      </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Silk Sonic                        </v>
+        <v>Mach-Hommy feat. Keisha Plum, Westside Gunn</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:39 </v>
+        <v xml:space="preserve">02:35 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1129,28 +1197,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">After Last Night     </v>
+        <v xml:space="preserve">Makrel Jaxon          </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II, James Fauntleroy, Stephen Bruner, Jonathan Yip, Ray Ronulas, Jeremy Reeves, Ray Charles McCullough II</v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Silk Sonic w/ Thundercat and Booty</v>
+        <v xml:space="preserve">Mach-Hommy                                 </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:09 </v>
+        <v xml:space="preserve">02:01 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1169,28 +1237,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Smokin Out the Window</v>
+        <v>The Stellar Ray Theory</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II                                                                                                       </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Silk Sonic                        </v>
+        <v xml:space="preserve">Mach-Hommy                                 </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:17 </v>
+        <v xml:space="preserve">03:15 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1209,28 +1277,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Put on a Smile       </v>
+        <v xml:space="preserve">Marie                 </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II, Kenny "Babyface" Edmonds                                                                             </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Silk Sonic                        </v>
+        <v xml:space="preserve">Mach-Hommy                                 </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:15 </v>
+        <v xml:space="preserve">02:49 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1249,28 +1317,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">777                  </v>
+        <v xml:space="preserve">Leta Yo (Skit)        </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II, Christopher Brody Brown                                                                              </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Silk Sonic                        </v>
+        <v xml:space="preserve">Mach-Hommy                                 </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:44 </v>
+        <v xml:space="preserve">00:34 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1289,28 +1357,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Skate                </v>
+        <v xml:space="preserve">Kriminel              </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II, James Fauntleroy, Domitille Degalle, J. D. Beck                                                      </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Silk Sonic                        </v>
+        <v xml:space="preserve">Mach-Hommy                                 </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:23 </v>
+        <v xml:space="preserve">02:36 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1329,28 +1397,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Blast Off            </v>
+        <v xml:space="preserve">Pen Rale              </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Bruno Mars, Brandon Anderson, Dernst Emile II                                                                                                       </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Silk Sonic                        </v>
+        <v xml:space="preserve">Mach-Hommy                                 </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:44 </v>
+        <v xml:space="preserve">01:41 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1362,35 +1430,35 @@
       </c>
       <c r="B14">
         <f>Sheet1!A11</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">Murder Czn            </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">Mach-Hommy feat. Westside Gunn             </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:28 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1402,35 +1470,35 @@
       </c>
       <c r="B15">
         <f>Sheet1!A12</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">Magnum Band           </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">Mach-Hommy feat. ThaGodFahim               </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:47 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1442,35 +1510,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">Rami                  </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">Mach-Hommy feat. Westside Gunn             </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:28 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1482,35 +1550,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">Kreyol (Skit)         </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">Mach-Hommy                                 </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">01:06 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1522,35 +1590,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">Au Revoir             </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">Mach-Hommy feat. Melanie Charles           </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:48 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1562,35 +1630,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">Blockchain            </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">Mach-Hommy                                 </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">01:47 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1602,35 +1670,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">Ten Boxes / Sin Eater </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">Mach-Hommy                                 </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve"> 2:50 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1649,21 +1717,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1689,21 +1757,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1729,21 +1797,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1769,21 +1837,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1809,21 +1877,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1849,21 +1917,21 @@
       </c>
       <c r="D26" t="str">
         <f>LEFTB(Sheet1!B23&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="str">
         <f>" "&amp;LEFTB(Sheet1!C23&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H26" t="str">
         <f>LEFTB(Sheet1!D23&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I26" s="4" t="s">
         <v>0</v>
@@ -1889,21 +1957,21 @@
       </c>
       <c r="D27" t="str">
         <f>LEFTB(Sheet1!B24&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="str">
         <f>" "&amp;LEFTB(Sheet1!C24&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H27" t="str">
         <f>LEFTB(Sheet1!D24&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I27" s="4" t="s">
         <v>0</v>
@@ -1929,21 +1997,21 @@
       </c>
       <c r="D28" t="str">
         <f>LEFTB(Sheet1!B25&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F28" t="str">
         <f>" "&amp;LEFTB(Sheet1!C25&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H28" t="str">
         <f>LEFTB(Sheet1!D25&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I28" s="4" t="s">
         <v>0</v>
@@ -1969,21 +2037,21 @@
       </c>
       <c r="D29" t="str">
         <f>LEFTB(Sheet1!B26&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E29" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F29" t="str">
         <f>" "&amp;LEFTB(Sheet1!C26&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G29" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H29" t="str">
         <f>LEFTB(Sheet1!D26&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I29" s="4" t="s">
         <v>0</v>
@@ -2009,21 +2077,21 @@
       </c>
       <c r="D30" t="str">
         <f>LEFTB(Sheet1!B27&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F30" t="str">
         <f>" "&amp;LEFTB(Sheet1!C27&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H30" t="str">
         <f>LEFTB(Sheet1!D27&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I30" s="4" t="s">
         <v>0</v>
@@ -2049,21 +2117,21 @@
       </c>
       <c r="D31" t="str">
         <f>LEFTB(Sheet1!B28&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F31" t="str">
         <f>" "&amp;LEFTB(Sheet1!C28&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H31" t="str">
         <f>LEFTB(Sheet1!D28&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I31" s="4" t="s">
         <v>0</v>
@@ -2089,21 +2157,21 @@
       </c>
       <c r="D32" t="str">
         <f>LEFTB(Sheet1!B29&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F32" t="str">
         <f>" "&amp;LEFTB(Sheet1!C29&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H32" t="str">
         <f>LEFTB(Sheet1!D29&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I32" s="4" t="s">
         <v>0</v>
@@ -2129,21 +2197,21 @@
       </c>
       <c r="D33" t="str">
         <f>LEFTB(Sheet1!B30&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F33" t="str">
         <f>" "&amp;LEFTB(Sheet1!C30&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve">         </v>
       </c>
       <c r="G33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H33" t="str">
         <f>LEFTB(Sheet1!D30&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I33" s="4" t="s">
         <v>0</v>
@@ -2173,11 +2241,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="45" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
@@ -2206,14 +2274,11 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="2">
-        <v>4.3750000000000004E-2</v>
+        <v>0.15208333333333332</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2225,16 +2290,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.16805555555555554</v>
+        <v>7.9166666666666663E-2</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2246,16 +2308,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15208333333333332</v>
+        <v>0.1076388888888889</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2267,16 +2326,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.17291666666666669</v>
+        <v>8.4027777777777771E-2</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2288,16 +2344,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
       <c r="E6" s="2">
-        <v>0.13680555555555554</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2309,16 +2363,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.17708333333333334</v>
+        <v>0.1173611111111111</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2329,17 +2380,14 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>777</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
+      <c r="B8" t="s">
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.11388888888888889</v>
+        <v>2.361111111111111E-2</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2351,16 +2399,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.14097222222222222</v>
+        <v>0.10833333333333334</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2372,16 +2417,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
       <c r="E10" s="2">
-        <v>0.19722222222222222</v>
+        <v>7.013888888888889E-2</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2389,57 +2431,133 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="E11" s="2"/>
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.14444444444444446</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="E12" s="2"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.11597222222222221</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="B13" s="5"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="C13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.10277777777777779</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4.5833333333333337E-2</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.15833333333333333</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="E16" s="2"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2">
+        <v>7.4305555555555555E-2</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="5:10">
-      <c r="E17" s="2"/>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="5:10">
+    <row r="18" spans="1:10">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -2447,7 +2565,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="5:10">
+    <row r="19" spans="1:10">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -2455,64 +2573,64 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="5:10">
+    <row r="20" spans="1:10">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="5:10">
+    <row r="21" spans="1:10">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="5:10">
+    <row r="22" spans="1:10">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="5:10">
+    <row r="23" spans="1:10">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="5:10">
+    <row r="24" spans="1:10">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="5:10">
+    <row r="25" spans="1:10">
       <c r="E25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="5:10">
+    <row r="26" spans="1:10">
       <c r="E26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="5:10">
+    <row r="27" spans="1:10">
       <c r="E27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="5:10">
+    <row r="28" spans="1:10">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="5:10">
+    <row r="29" spans="1:10">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="5:10">
+    <row r="30" spans="1:10">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="5:10">
+    <row r="31" spans="1:10">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="5:10">
+    <row r="32" spans="1:10">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="9:9">

</xml_diff>

<commit_message>
02111600 added review vs ir
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="machhommy1" localSheetId="0">Sheet1!$A$1:$E$17</definedName>
-    <definedName name="machhommy1" localSheetId="2">Sheet3!$A$1:$E$17</definedName>
+    <definedName name="isaiahrashad1" localSheetId="0">Sheet1!$A$1:$E$17</definedName>
+    <definedName name="isaiahrashad1" localSheetId="2">Sheet3!$A$1:$E$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/machhommy1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/isaiahrashad1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/machhommy1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="https://bm.planetky.com/isaiahrashad1.htm" htmlTables="1">
       <tables count="1">
         <x v="5"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="49">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -75,70 +75,130 @@
     <t>Composer</t>
   </si>
   <si>
-    <t>The 26th Letter</t>
-  </si>
-  <si>
-    <t>Mach-Hommy</t>
-  </si>
-  <si>
-    <t>No Blood No Sweat</t>
-  </si>
-  <si>
-    <t>Folie Á Deux</t>
-  </si>
-  <si>
-    <t>Mach-Hommy feat. Keisha Plum, Westside Gunn</t>
-  </si>
-  <si>
-    <t>Makrel Jaxon</t>
-  </si>
-  <si>
-    <t>The Stellar Ray Theory</t>
-  </si>
-  <si>
-    <t>Marie</t>
-  </si>
-  <si>
-    <t>Leta Yo (Skit)</t>
-  </si>
-  <si>
-    <t>Kriminel</t>
-  </si>
-  <si>
-    <t>Pen Rale</t>
-  </si>
-  <si>
-    <t>Murder Czn</t>
-  </si>
-  <si>
-    <t>Mach-Hommy feat. Westside Gunn</t>
-  </si>
-  <si>
-    <t>Magnum Band</t>
-  </si>
-  <si>
-    <t>Mach-Hommy feat. ThaGodFahim</t>
-  </si>
-  <si>
-    <t>Rami</t>
-  </si>
-  <si>
-    <t>Kreyol (Skit)</t>
-  </si>
-  <si>
-    <t>Au Revoir</t>
-  </si>
-  <si>
-    <t>Mach-Hommy feat. Melanie Charles</t>
-  </si>
-  <si>
-    <t>Blockchain</t>
-  </si>
-  <si>
-    <t>Ten Boxes / Sin Eater</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2:50</t>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Darkseid</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Devin Williams, Eliot Dubock</t>
+  </si>
+  <si>
+    <t>Isaiah Rashad</t>
+  </si>
+  <si>
+    <t>From the Garden</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Symere Woods, Kalon Berry, Keanu Torres, Solal Tong Cuong, Freddie Jefferson III</t>
+  </si>
+  <si>
+    <t>Isaiah Rashad feat. Lil Uzi Vert</t>
+  </si>
+  <si>
+    <t>RIP Young</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Kalon Berry, Patrick Houston, Paul Beauregard, Jordan Houston, Jorge Barreiro</t>
+  </si>
+  <si>
+    <t>Lay wit Ya</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Patavious Isom, Kameron Cole, Paul Beauregard, J. Houston, James Johnson Jr., LeRoi Johnson</t>
+  </si>
+  <si>
+    <t>Isaiah Rashad feat. Duke Deuce</t>
+  </si>
+  <si>
+    <t>Claymore</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Christopher Smith Jr., Kalon Berry, Jason Pounds, Benjamin Tolbert</t>
+  </si>
+  <si>
+    <t>Isaiah Rashad feat. Smino</t>
+  </si>
+  <si>
+    <t>Headshots (4r da Locals)</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Kameron Cole, Henry Fagenson, Piero Piccioni</t>
+  </si>
+  <si>
+    <t>All Herb</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Amindi Frost, Devin Williams</t>
+  </si>
+  <si>
+    <t>Isaiah Rashad feat. Amindi</t>
+  </si>
+  <si>
+    <t>Hey Mista</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Kalon Berry</t>
+  </si>
+  <si>
+    <t>True Story</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Johnny McKinzie Jr., James Sidhoo, Devin Williams, Kelvin Wooten</t>
+  </si>
+  <si>
+    <t>Isaiah Rashad feat. Jay Rock, Jay Worthy</t>
+  </si>
+  <si>
+    <t>Wat U Sed</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Jaylah Hickmon, Kalon Berry, Amaire Johnson, Rory Behr</t>
+  </si>
+  <si>
+    <t>Isaiah Rashad feat. Doechii, Kal Banx</t>
+  </si>
+  <si>
+    <t>Don't Shoot</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Kalon Berry, Rory Behr</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Kevin Adams Jr., Devin Williams, Kalon Berry, Sam Yun</t>
+  </si>
+  <si>
+    <t>Isaiah Rashad feat. YGTUT</t>
+  </si>
+  <si>
+    <t>9-3 Freestyle</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Devin Williams, Kalon Berry</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Kenneth Blume III, Kalon Berry, Solana Rowe, Ricardo Valentine Jr.</t>
+  </si>
+  <si>
+    <t>Isaiah Rashad feat. SZA, 6lack</t>
+  </si>
+  <si>
+    <t>THIB</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Freddie Jefferson III, Calvin Tarvin, Melissa Elliott, Timothy Mosley, Margaret Peebles, Bernard Miller, Donald Bryant, Robert Barnett, Patrick Brown, Thomas Callaway, Cameron Gipp, William Knighton Jr. Raymon Murray, Rico Wade</t>
+  </si>
+  <si>
+    <t>HB2U</t>
+  </si>
+  <si>
+    <t>Isaiah McClain, Russell Scott-Wood, Tyran Donaldson II, Kalon Berry, Rory Behr, William Stewart II</t>
   </si>
 </sst>
 </file>
@@ -233,11 +293,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="machhommy1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="isaiahrashad1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="machhommy1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="isaiahrashad1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,10 +605,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" customWidth="1"/>
-    <col min="4" max="4" width="45" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="37.5546875" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
@@ -558,6 +618,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -576,13 +639,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>0.15208333333333332</v>
+        <v>8.819444444444445E-2</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -594,13 +660,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
-        <v>7.9166666666666663E-2</v>
+        <v>0.13125000000000001</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -612,13 +681,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
       <c r="E4" s="2">
-        <v>0.1076388888888889</v>
+        <v>0.10972222222222222</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -630,13 +702,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2">
-        <v>8.4027777777777771E-2</v>
+        <v>0.14027777777777778</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -648,14 +723,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.12916666666666668</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -667,13 +744,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2">
-        <v>0.1173611111111111</v>
+        <v>0.13402777777777777</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -685,13 +765,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2">
-        <v>2.361111111111111E-2</v>
+        <v>0.15555555555555556</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -703,13 +786,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
-        <v>0.10833333333333334</v>
+        <v>8.0555555555555561E-2</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -721,13 +807,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2">
-        <v>7.013888888888889E-2</v>
+        <v>0.15763888888888888</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -739,13 +828,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2">
-        <v>0.14444444444444446</v>
+        <v>0.12291666666666667</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -757,13 +849,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2">
-        <v>0.11597222222222221</v>
+        <v>9.7916666666666666E-2</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -775,14 +870,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E13" s="5">
-        <v>0.10277777777777779</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
@@ -794,13 +891,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2">
-        <v>4.5833333333333337E-2</v>
+        <v>7.3611111111111113E-2</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -812,13 +912,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E15" s="2">
-        <v>0.15833333333333333</v>
+        <v>0.13958333333333334</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -830,13 +933,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2">
-        <v>7.4305555555555555E-2</v>
+        <v>0.1076388888888889</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -848,13 +954,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.23958333333333334</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -971,15 +1080,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>8</v>
+        <v>243</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -999,21 +1108,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                 </v>
+        <v xml:space="preserve"> Title                   </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Compose</v>
+        <v xml:space="preserve"> Composers                                                                                                                                                                                                                                         </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                                  </v>
+        <v xml:space="preserve"> Performer                               </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1038,21 +1147,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">---------------------- </v>
+        <v xml:space="preserve">------------------------ </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> -------- </v>
+        <v xml:space="preserve"> --------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------- </v>
+        <v xml:space="preserve"> ---------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1077,28 +1186,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">The 26th Letter       </v>
+        <v xml:space="preserve">Darkseid                </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Devin Williams, Eliot Dubock                                                                                                                                                                                                       </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy                                 </v>
+        <v xml:space="preserve">Isaiah Rashad                           </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:39 </v>
+        <v xml:space="preserve">02:07 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1117,28 +1226,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">No Blood No Sweat     </v>
+        <v xml:space="preserve">From the Garden         </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Symere Woods, Kalon Berry, Keanu Torres, Solal Tong Cuong, Freddie Jefferson III                                                                                                                                                   </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy                                 </v>
+        <v xml:space="preserve">Isaiah Rashad feat. Lil Uzi Vert        </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:54 </v>
+        <v xml:space="preserve">03:09 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1157,28 +1266,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Folie Á Deux         </v>
+        <v xml:space="preserve">RIP Young               </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Kalon Berry, Patrick Houston, Paul Beauregard, Jordan Houston, Jorge Barreiro                                                                                                                                                      </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Mach-Hommy feat. Keisha Plum, Westside Gunn</v>
+        <v xml:space="preserve">Isaiah Rashad                           </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:35 </v>
+        <v xml:space="preserve">02:38 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1197,28 +1306,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Makrel Jaxon          </v>
+        <v xml:space="preserve">Lay wit Ya              </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Patavious Isom, Kameron Cole, Paul Beauregard, J. Houston, James Johnson Jr., LeRoi Johnson                                                                                                                                        </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy                                 </v>
+        <v xml:space="preserve">Isaiah Rashad feat. Duke Deuce          </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:01 </v>
+        <v xml:space="preserve">03:22 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1237,28 +1346,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>The Stellar Ray Theory</v>
+        <v xml:space="preserve">Claymore                </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Christopher Smith Jr., Kalon Berry, Jason Pounds, Benjamin Tolbert                                                                                                                                                                 </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy                                 </v>
+        <v xml:space="preserve">Isaiah Rashad feat. Smino               </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:15 </v>
+        <v xml:space="preserve">03:06 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1277,28 +1386,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Marie                 </v>
+        <v>Headshots (4r da Locals)</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Kameron Cole, Henry Fagenson, Piero Piccioni                                                                                                                                                                                       </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy                                 </v>
+        <v xml:space="preserve">Isaiah Rashad                           </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:49 </v>
+        <v xml:space="preserve">03:13 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1317,28 +1426,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Leta Yo (Skit)        </v>
+        <v xml:space="preserve">All Herb                </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Amindi Frost, Devin Williams                                                                                                                                                                                                       </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy                                 </v>
+        <v xml:space="preserve">Isaiah Rashad feat. Amindi              </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:34 </v>
+        <v xml:space="preserve">03:44 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1357,28 +1466,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Kriminel              </v>
+        <v xml:space="preserve">Hey Mista               </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Kalon Berry                                                                                                                                                                                                                        </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy                                 </v>
+        <v xml:space="preserve">Isaiah Rashad                           </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:36 </v>
+        <v xml:space="preserve">01:56 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1397,28 +1506,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Pen Rale              </v>
+        <v xml:space="preserve">True Story              </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Johnny McKinzie Jr., James Sidhoo, Devin Williams, Kelvin Wooten                                                                                                                                                                   </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy                                 </v>
+        <v>Isaiah Rashad feat. Jay Rock, Jay Worthy</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:41 </v>
+        <v xml:space="preserve">03:47 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1437,28 +1546,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Murder Czn            </v>
+        <v xml:space="preserve">Wat U Sed               </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Jaylah Hickmon, Kalon Berry, Amaire Johnson, Rory Behr                                                                                                                                                                             </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy feat. Westside Gunn             </v>
+        <v xml:space="preserve">Isaiah Rashad feat. Doechii, Kal Banx   </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:28 </v>
+        <v xml:space="preserve">02:57 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1477,28 +1586,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Magnum Band           </v>
+        <v xml:space="preserve">Don't Shoot             </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Kalon Berry, Rory Behr                                                                                                                                                                                                             </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy feat. ThaGodFahim               </v>
+        <v xml:space="preserve">Isaiah Rashad                           </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:47 </v>
+        <v xml:space="preserve">02:21 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1517,28 +1626,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Rami                  </v>
+        <v xml:space="preserve">Chad                    </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Kevin Adams Jr., Devin Williams, Kalon Berry, Sam Yun                                                                                                                                                                              </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy feat. Westside Gunn             </v>
+        <v xml:space="preserve">Isaiah Rashad feat. YGTUT               </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:28 </v>
+        <v xml:space="preserve">02:40 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1557,28 +1666,28 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Kreyol (Skit)         </v>
+        <v xml:space="preserve">9-3 Freestyle           </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Devin Williams, Kalon Berry                                                                                                                                                                                                        </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy                                 </v>
+        <v xml:space="preserve">Isaiah Rashad                           </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:06 </v>
+        <v xml:space="preserve">01:46 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1597,28 +1706,28 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Au Revoir             </v>
+        <v xml:space="preserve">Score                   </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Kenneth Blume III, Kalon Berry, Solana Rowe, Ricardo Valentine Jr.                                                                                                                                                                 </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy feat. Melanie Charles           </v>
+        <v xml:space="preserve">Isaiah Rashad feat. SZA, 6lack          </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:48 </v>
+        <v xml:space="preserve">03:21 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1637,28 +1746,28 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Blockchain            </v>
+        <v xml:space="preserve">THIB                    </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Freddie Jefferson III, Calvin Tarvin, Melissa Elliott, Timothy Mosley, Margaret Peebles, Bernard Miller, Donald Bryant, Robert Barnett, Patrick Brown, Thomas Callaway, Cameron Gipp, William Knighton Jr. Raymon Murray, Rico Wade</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy                                 </v>
+        <v xml:space="preserve">Isaiah Rashad                           </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:47 </v>
+        <v xml:space="preserve">02:35 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1677,28 +1786,28 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Ten Boxes / Sin Eater </v>
+        <v xml:space="preserve">HB2U                    </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve"> Isaiah McClain, Russell Scott-Wood, Tyran Donaldson II, Kalon Berry, Rory Behr, William Stewart II                                                                                                                                                 </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Mach-Hommy                                 </v>
+        <v xml:space="preserve">Isaiah Rashad                           </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve"> 2:50 </v>
+        <v xml:space="preserve">05:45 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1717,21 +1826,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1757,21 +1866,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1797,21 +1906,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1837,21 +1946,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1877,21 +1986,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1917,21 +2026,21 @@
       </c>
       <c r="D26" t="str">
         <f>LEFTB(Sheet1!B23&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="str">
         <f>" "&amp;LEFTB(Sheet1!C23&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H26" t="str">
         <f>LEFTB(Sheet1!D23&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I26" s="4" t="s">
         <v>0</v>
@@ -1957,21 +2066,21 @@
       </c>
       <c r="D27" t="str">
         <f>LEFTB(Sheet1!B24&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="str">
         <f>" "&amp;LEFTB(Sheet1!C24&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H27" t="str">
         <f>LEFTB(Sheet1!D24&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I27" s="4" t="s">
         <v>0</v>
@@ -1997,21 +2106,21 @@
       </c>
       <c r="D28" t="str">
         <f>LEFTB(Sheet1!B25&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F28" t="str">
         <f>" "&amp;LEFTB(Sheet1!C25&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H28" t="str">
         <f>LEFTB(Sheet1!D25&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I28" s="4" t="s">
         <v>0</v>
@@ -2037,21 +2146,21 @@
       </c>
       <c r="D29" t="str">
         <f>LEFTB(Sheet1!B26&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E29" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F29" t="str">
         <f>" "&amp;LEFTB(Sheet1!C26&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G29" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H29" t="str">
         <f>LEFTB(Sheet1!D26&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I29" s="4" t="s">
         <v>0</v>
@@ -2077,21 +2186,21 @@
       </c>
       <c r="D30" t="str">
         <f>LEFTB(Sheet1!B27&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F30" t="str">
         <f>" "&amp;LEFTB(Sheet1!C27&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H30" t="str">
         <f>LEFTB(Sheet1!D27&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I30" s="4" t="s">
         <v>0</v>
@@ -2117,21 +2226,21 @@
       </c>
       <c r="D31" t="str">
         <f>LEFTB(Sheet1!B28&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F31" t="str">
         <f>" "&amp;LEFTB(Sheet1!C28&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H31" t="str">
         <f>LEFTB(Sheet1!D28&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I31" s="4" t="s">
         <v>0</v>
@@ -2157,21 +2266,21 @@
       </c>
       <c r="D32" t="str">
         <f>LEFTB(Sheet1!B29&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F32" t="str">
         <f>" "&amp;LEFTB(Sheet1!C29&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H32" t="str">
         <f>LEFTB(Sheet1!D29&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I32" s="4" t="s">
         <v>0</v>
@@ -2197,21 +2306,21 @@
       </c>
       <c r="D33" t="str">
         <f>LEFTB(Sheet1!B30&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F33" t="str">
         <f>" "&amp;LEFTB(Sheet1!C30&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">         </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H33" t="str">
         <f>LEFTB(Sheet1!D30&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I33" s="4" t="s">
         <v>0</v>
@@ -2241,10 +2350,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" customWidth="1"/>
-    <col min="4" max="4" width="45" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="37.5546875" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
@@ -2254,6 +2363,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -2272,13 +2384,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>0.15208333333333332</v>
+        <v>8.819444444444445E-2</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2290,13 +2405,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
-        <v>7.9166666666666663E-2</v>
+        <v>0.13125000000000001</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2308,13 +2426,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
       <c r="E4" s="2">
-        <v>0.1076388888888889</v>
+        <v>0.10972222222222222</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2326,13 +2447,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2">
-        <v>8.4027777777777771E-2</v>
+        <v>0.14027777777777778</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2344,14 +2468,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.12916666666666668</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2363,13 +2489,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2">
-        <v>0.1173611111111111</v>
+        <v>0.13402777777777777</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2381,13 +2510,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2">
-        <v>2.361111111111111E-2</v>
+        <v>0.15555555555555556</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2399,13 +2531,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
-        <v>0.10833333333333334</v>
+        <v>8.0555555555555561E-2</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2417,13 +2552,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2">
-        <v>7.013888888888889E-2</v>
+        <v>0.15763888888888888</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2435,13 +2573,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2">
-        <v>0.14444444444444446</v>
+        <v>0.12291666666666667</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2453,13 +2594,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2">
-        <v>0.11597222222222221</v>
+        <v>9.7916666666666666E-2</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2471,14 +2615,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E13" s="5">
-        <v>0.10277777777777779</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="2"/>
@@ -2490,13 +2636,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2">
-        <v>4.5833333333333337E-2</v>
+        <v>7.3611111111111113E-2</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2508,13 +2657,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E15" s="2">
-        <v>0.15833333333333333</v>
+        <v>0.13958333333333334</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -2526,13 +2678,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2">
-        <v>7.4305555555555555E-2</v>
+        <v>0.1076388888888889</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -2544,13 +2699,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.23958333333333334</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>

</xml_diff>